<commit_message>
Added simplified weather excel
</commit_message>
<xml_diff>
--- a/simpleWeather.xlsx
+++ b/simpleWeather.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Foglio1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Foglio1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="162913" fullCalcOnLoad="1"/>
@@ -210,12 +210,13 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -292,84 +293,17 @@
     <xf numFmtId="0" fontId="2" fillId="23" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="25" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>5</col>
@@ -384,13 +318,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -409,13 +343,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -434,13 +368,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId3"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -459,13 +393,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId4"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -484,13 +418,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId5"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -509,13 +443,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId6"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -534,13 +468,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId7"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId7"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -559,13 +493,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId8"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId8"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -584,13 +518,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId9"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId9"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -609,13 +543,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId10"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId10"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -634,13 +568,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId11"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId11"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -659,13 +593,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId12"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId12"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -684,13 +618,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId13"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId13"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -709,13 +643,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId14"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId14"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -734,13 +668,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId15"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId15"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -759,13 +693,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId16"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId16"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -784,13 +718,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId17"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId17"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -809,13 +743,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId18"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId18"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -834,13 +768,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId19"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId19"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -859,13 +793,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId20"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId20"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -884,13 +818,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId21"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId21"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -909,13 +843,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId22"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId22"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -934,13 +868,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId23"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId23"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -959,13 +893,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId24"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId24"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -984,13 +918,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId25"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId25"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1009,13 +943,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId26"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId26"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1034,13 +968,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId27"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId27"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1059,13 +993,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId28"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId28"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1084,13 +1018,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId29"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId29"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1109,13 +1043,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId30"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId30"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1134,13 +1068,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId31"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId31"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1159,13 +1093,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId32"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId32"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1184,13 +1118,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId33"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId33"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1209,13 +1143,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId34"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId34"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1234,13 +1168,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId35"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId35"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1259,13 +1193,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId36"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId36"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1284,13 +1218,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId37"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId37"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1309,13 +1243,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId38"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId38"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1334,13 +1268,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId39"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId39"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1359,13 +1293,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId40"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId40"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1384,13 +1318,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId41"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId41"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1409,13 +1343,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId42"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId42"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1434,13 +1368,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId43"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId43"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1459,13 +1393,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId44"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId44"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1735,7 +1669,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -1814,27 +1748,27 @@
     <row r="2">
       <c r="A2" s="61" t="inlineStr">
         <is>
-          <t>2021-09-07 03:00</t>
+          <t>2021-10-06 03:00</t>
         </is>
       </c>
       <c r="B2" s="65" t="n">
-        <v>21</v>
-      </c>
-      <c r="C2" s="64" t="n">
-        <v>15</v>
-      </c>
-      <c r="D2" s="67" t="n">
-        <v>69</v>
+        <v>20</v>
+      </c>
+      <c r="C2" s="76" t="n">
+        <v>18</v>
+      </c>
+      <c r="D2" s="69" t="n">
+        <v>86</v>
       </c>
       <c r="E2" s="66" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F2" s="61" t="n">
-        <v>106</v>
-      </c>
-      <c r="G2" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
+        <v>305</v>
+      </c>
+      <c r="G2" s="72" t="inlineStr">
+        <is>
+          <t>0.0001168</t>
         </is>
       </c>
       <c r="H2" s="66" t="inlineStr">
@@ -1852,46 +1786,46 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K2" s="68" t="inlineStr">
-        <is>
-          <t>32.3</t>
+      <c r="K2" s="61" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L2" s="68" t="inlineStr">
         <is>
-          <t>54.1</t>
-        </is>
-      </c>
-      <c r="M2" s="73" t="inlineStr">
-        <is>
-          <t>75.1</t>
+          <t>44.1</t>
+        </is>
+      </c>
+      <c r="M2" s="74" t="inlineStr">
+        <is>
+          <t>100</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="61" t="inlineStr">
         <is>
-          <t>2021-09-07 06:00</t>
+          <t>2021-10-06 06:00</t>
         </is>
       </c>
       <c r="B3" s="65" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="64" t="n">
-        <v>15</v>
-      </c>
-      <c r="D3" s="67" t="n">
-        <v>64</v>
+        <v>16</v>
+      </c>
+      <c r="D3" s="69" t="n">
+        <v>77</v>
       </c>
       <c r="E3" s="66" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F3" s="61" t="n">
-        <v>132</v>
-      </c>
-      <c r="G3" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
+        <v>249</v>
+      </c>
+      <c r="G3" s="72" t="inlineStr">
+        <is>
+          <t>3.84e-05</t>
         </is>
       </c>
       <c r="H3" s="66" t="inlineStr">
@@ -1909,42 +1843,42 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K3" s="70" t="inlineStr">
-        <is>
-          <t>16.4</t>
+      <c r="K3" s="66" t="inlineStr">
+        <is>
+          <t>0.1</t>
         </is>
       </c>
       <c r="L3" s="75" t="inlineStr">
         <is>
-          <t>27.1</t>
-        </is>
-      </c>
-      <c r="M3" s="61" t="inlineStr">
-        <is>
-          <t>85</t>
+          <t>23.2</t>
+        </is>
+      </c>
+      <c r="M3" s="68" t="inlineStr">
+        <is>
+          <t>53.3</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="61" t="inlineStr">
         <is>
-          <t>2021-09-07 09:00</t>
+          <t>2021-10-06 09:00</t>
         </is>
       </c>
       <c r="B4" s="63" t="n">
-        <v>27</v>
-      </c>
-      <c r="C4" s="63" t="n">
-        <v>12</v>
+        <v>25</v>
+      </c>
+      <c r="C4" s="64" t="n">
+        <v>14</v>
       </c>
       <c r="D4" s="65" t="n">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="E4" s="66" t="n">
         <v>2</v>
       </c>
       <c r="F4" s="61" t="n">
-        <v>72</v>
+        <v>243</v>
       </c>
       <c r="G4" s="66" t="inlineStr">
         <is>
@@ -1966,9 +1900,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K4" s="66" t="inlineStr">
-        <is>
-          <t>5</t>
+      <c r="K4" s="61" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L4" s="61" t="inlineStr">
@@ -1976,16 +1910,16 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M4" s="75" t="inlineStr">
-        <is>
-          <t>30</t>
+      <c r="M4" s="66" t="inlineStr">
+        <is>
+          <t>1.3</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="61" t="inlineStr">
         <is>
-          <t>2021-09-07 12:00</t>
+          <t>2021-10-06 12:00</t>
         </is>
       </c>
       <c r="B5" s="63" t="n">
@@ -1998,14 +1932,14 @@
         <v>42</v>
       </c>
       <c r="E5" s="66" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F5" s="61" t="n">
-        <v>33</v>
-      </c>
-      <c r="G5" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
+        <v>282</v>
+      </c>
+      <c r="G5" s="72" t="inlineStr">
+        <is>
+          <t>3.2e-06</t>
         </is>
       </c>
       <c r="H5" s="66" t="inlineStr">
@@ -2023,42 +1957,42 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K5" s="71" t="inlineStr">
-        <is>
-          <t>7.1</t>
-        </is>
-      </c>
-      <c r="L5" s="61" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M5" s="68" t="inlineStr">
-        <is>
-          <t>59.5</t>
+      <c r="K5" s="66" t="inlineStr">
+        <is>
+          <t>4.1</t>
+        </is>
+      </c>
+      <c r="L5" s="66" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="M5" s="75" t="inlineStr">
+        <is>
+          <t>25.9</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="61" t="inlineStr">
         <is>
-          <t>2021-09-07 15:00</t>
+          <t>2021-10-06 15:00</t>
         </is>
       </c>
       <c r="B6" s="63" t="n">
         <v>26</v>
       </c>
-      <c r="C6" s="64" t="n">
-        <v>13</v>
+      <c r="C6" s="63" t="n">
+        <v>12</v>
       </c>
       <c r="D6" s="65" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E6" s="66" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F6" s="61" t="n">
-        <v>97</v>
+        <v>266</v>
       </c>
       <c r="G6" s="66" t="inlineStr">
         <is>
@@ -2080,9 +2014,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K6" s="70" t="inlineStr">
-        <is>
-          <t>10.4</t>
+      <c r="K6" s="61" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L6" s="61" t="inlineStr">
@@ -2090,36 +2024,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M6" s="73" t="inlineStr">
-        <is>
-          <t>61.1</t>
+      <c r="M6" s="74" t="inlineStr">
+        <is>
+          <t>99.8</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="61" t="inlineStr">
         <is>
-          <t>2021-09-07 18:00</t>
+          <t>2021-10-06 18:00</t>
         </is>
       </c>
       <c r="B7" s="65" t="n">
         <v>22</v>
       </c>
       <c r="C7" s="64" t="n">
-        <v>13</v>
-      </c>
-      <c r="D7" s="65" t="n">
-        <v>55</v>
+        <v>15</v>
+      </c>
+      <c r="D7" s="67" t="n">
+        <v>67</v>
       </c>
       <c r="E7" s="66" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F7" s="61" t="n">
-        <v>79</v>
-      </c>
-      <c r="G7" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
+        <v>293</v>
+      </c>
+      <c r="G7" s="72" t="inlineStr">
+        <is>
+          <t>8e-07</t>
         </is>
       </c>
       <c r="H7" s="66" t="inlineStr">
@@ -2137,46 +2071,46 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K7" s="71" t="inlineStr">
-        <is>
-          <t>5.2</t>
-        </is>
-      </c>
-      <c r="L7" s="61" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M7" s="73" t="inlineStr">
-        <is>
-          <t>78.9</t>
+      <c r="K7" s="61" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L7" s="66" t="inlineStr">
+        <is>
+          <t>2.8</t>
+        </is>
+      </c>
+      <c r="M7" s="74" t="inlineStr">
+        <is>
+          <t>89.8</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="61" t="inlineStr">
         <is>
-          <t>2021-09-07 21:00</t>
+          <t>2021-10-06 21:00</t>
         </is>
       </c>
       <c r="B8" s="65" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="64" t="n">
-        <v>15</v>
-      </c>
-      <c r="D8" s="67" t="n">
-        <v>62</v>
+        <v>16</v>
+      </c>
+      <c r="D8" s="69" t="n">
+        <v>72</v>
       </c>
       <c r="E8" s="66" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F8" s="61" t="n">
-        <v>67</v>
-      </c>
-      <c r="G8" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
+        <v>284</v>
+      </c>
+      <c r="G8" s="72" t="inlineStr">
+        <is>
+          <t>6e-05</t>
         </is>
       </c>
       <c r="H8" s="66" t="inlineStr">
@@ -2199,37 +2133,37 @@
           <t>0</t>
         </is>
       </c>
-      <c r="L8" s="61" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M8" s="66" t="inlineStr">
-        <is>
-          <t>1.1</t>
+      <c r="L8" s="71" t="inlineStr">
+        <is>
+          <t>8.1</t>
+        </is>
+      </c>
+      <c r="M8" s="61" t="inlineStr">
+        <is>
+          <t>82.7</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="61" t="inlineStr">
         <is>
-          <t>2021-09-08 00:00</t>
+          <t>2021-10-07 00:00</t>
         </is>
       </c>
       <c r="B9" s="65" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="64" t="n">
-        <v>14</v>
-      </c>
-      <c r="D9" s="67" t="n">
-        <v>62</v>
+        <v>16</v>
+      </c>
+      <c r="D9" s="69" t="n">
+        <v>71</v>
       </c>
       <c r="E9" s="66" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F9" s="61" t="n">
-        <v>95</v>
+        <v>262</v>
       </c>
       <c r="G9" s="66" t="inlineStr">
         <is>
@@ -2251,51 +2185,51 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K9" s="70" t="inlineStr">
-        <is>
-          <t>13.2</t>
-        </is>
-      </c>
-      <c r="L9" s="66" t="inlineStr">
-        <is>
-          <t>1.4</t>
-        </is>
-      </c>
-      <c r="M9" s="66" t="inlineStr">
-        <is>
-          <t>0.5</t>
+      <c r="K9" s="66" t="inlineStr">
+        <is>
+          <t>2.1</t>
+        </is>
+      </c>
+      <c r="L9" s="68" t="inlineStr">
+        <is>
+          <t>38.8</t>
+        </is>
+      </c>
+      <c r="M9" s="73" t="inlineStr">
+        <is>
+          <t>76.2</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="61" t="inlineStr">
         <is>
-          <t>2021-09-08 03:00</t>
+          <t>2021-10-07 03:00</t>
         </is>
       </c>
       <c r="B10" s="65" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C10" s="64" t="n">
-        <v>14</v>
-      </c>
-      <c r="D10" s="67" t="n">
-        <v>67</v>
+        <v>16</v>
+      </c>
+      <c r="D10" s="69" t="n">
+        <v>86</v>
       </c>
       <c r="E10" s="66" t="n">
         <v>2</v>
       </c>
       <c r="F10" s="61" t="n">
-        <v>94</v>
-      </c>
-      <c r="G10" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H10" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
+        <v>221</v>
+      </c>
+      <c r="G10" s="72" t="inlineStr">
+        <is>
+          <t>0.0007136</t>
+        </is>
+      </c>
+      <c r="H10" s="65" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="I10" s="66" t="inlineStr">
@@ -2308,51 +2242,51 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K10" s="68" t="inlineStr">
-        <is>
-          <t>54.8</t>
-        </is>
-      </c>
-      <c r="L10" s="75" t="inlineStr">
-        <is>
-          <t>26.8</t>
-        </is>
-      </c>
-      <c r="M10" s="61" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K10" s="66" t="inlineStr">
+        <is>
+          <t>1.2</t>
+        </is>
+      </c>
+      <c r="L10" s="70" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="M10" s="74" t="inlineStr">
+        <is>
+          <t>100</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="61" t="inlineStr">
         <is>
-          <t>2021-09-08 06:00</t>
+          <t>2021-10-07 06:00</t>
         </is>
       </c>
       <c r="B11" s="65" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C11" s="64" t="n">
         <v>15</v>
       </c>
-      <c r="D11" s="67" t="n">
-        <v>61</v>
+      <c r="D11" s="69" t="n">
+        <v>84</v>
       </c>
       <c r="E11" s="66" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F11" s="61" t="n">
-        <v>108</v>
-      </c>
-      <c r="G11" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H11" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
+        <v>140</v>
+      </c>
+      <c r="G11" s="72" t="inlineStr">
+        <is>
+          <t>0.0008936</t>
+        </is>
+      </c>
+      <c r="H11" s="65" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="I11" s="66" t="inlineStr">
@@ -2367,40 +2301,40 @@
       </c>
       <c r="K11" s="75" t="inlineStr">
         <is>
-          <t>29.9</t>
-        </is>
-      </c>
-      <c r="L11" s="70" t="inlineStr">
-        <is>
-          <t>13.4</t>
-        </is>
-      </c>
-      <c r="M11" s="61" t="inlineStr">
-        <is>
-          <t>0</t>
+          <t>22.4</t>
+        </is>
+      </c>
+      <c r="L11" s="75" t="inlineStr">
+        <is>
+          <t>23.7</t>
+        </is>
+      </c>
+      <c r="M11" s="74" t="inlineStr">
+        <is>
+          <t>99.1</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="61" t="inlineStr">
         <is>
-          <t>2021-09-08 09:00</t>
-        </is>
-      </c>
-      <c r="B12" s="63" t="n">
-        <v>26</v>
-      </c>
-      <c r="C12" s="64" t="n">
-        <v>13</v>
+          <t>2021-10-07 09:00</t>
+        </is>
+      </c>
+      <c r="B12" s="65" t="n">
+        <v>22</v>
+      </c>
+      <c r="C12" s="63" t="n">
+        <v>12</v>
       </c>
       <c r="D12" s="65" t="n">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="E12" s="66" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F12" s="61" t="n">
-        <v>84</v>
+        <v>197</v>
       </c>
       <c r="G12" s="66" t="inlineStr">
         <is>
@@ -2422,46 +2356,46 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K12" s="66" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="L12" s="66" t="inlineStr">
-        <is>
-          <t>4.6</t>
-        </is>
-      </c>
-      <c r="M12" s="61" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K12" s="75" t="inlineStr">
+        <is>
+          <t>25.4</t>
+        </is>
+      </c>
+      <c r="L12" s="75" t="inlineStr">
+        <is>
+          <t>28.5</t>
+        </is>
+      </c>
+      <c r="M12" s="66" t="inlineStr">
+        <is>
+          <t>1.7</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="61" t="inlineStr">
         <is>
-          <t>2021-09-08 12:00</t>
+          <t>2021-10-07 12:00</t>
         </is>
       </c>
       <c r="B13" s="63" t="n">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C13" s="63" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13" s="65" t="n">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E13" s="66" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F13" s="61" t="n">
-        <v>79</v>
-      </c>
-      <c r="G13" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
+        <v>222</v>
+      </c>
+      <c r="G13" s="72" t="inlineStr">
+        <is>
+          <t>1.28e-05</t>
         </is>
       </c>
       <c r="H13" s="66" t="inlineStr">
@@ -2479,46 +2413,46 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K13" s="66" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="L13" s="66" t="inlineStr">
-        <is>
-          <t>4.8</t>
-        </is>
-      </c>
-      <c r="M13" s="61" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K13" s="70" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="L13" s="70" t="inlineStr">
+        <is>
+          <t>14.3</t>
+        </is>
+      </c>
+      <c r="M13" s="66" t="inlineStr">
+        <is>
+          <t>0.8</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="61" t="inlineStr">
         <is>
-          <t>2021-09-08 15:00</t>
-        </is>
-      </c>
-      <c r="B14" s="63" t="n">
-        <v>25</v>
+          <t>2021-10-07 15:00</t>
+        </is>
+      </c>
+      <c r="B14" s="65" t="n">
+        <v>22</v>
       </c>
       <c r="C14" s="63" t="n">
         <v>11</v>
       </c>
       <c r="D14" s="65" t="n">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="E14" s="66" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F14" s="61" t="n">
-        <v>319</v>
-      </c>
-      <c r="G14" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
+        <v>284</v>
+      </c>
+      <c r="G14" s="72" t="inlineStr">
+        <is>
+          <t>1.28e-05</t>
         </is>
       </c>
       <c r="H14" s="66" t="inlineStr">
@@ -2536,46 +2470,46 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K14" s="66" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="L14" s="66" t="inlineStr">
-        <is>
-          <t>2.9</t>
-        </is>
-      </c>
-      <c r="M14" s="66" t="inlineStr">
-        <is>
-          <t>2</t>
+      <c r="K14" s="74" t="inlineStr">
+        <is>
+          <t>86.4</t>
+        </is>
+      </c>
+      <c r="L14" s="61" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M14" s="61" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="61" t="inlineStr">
         <is>
-          <t>2021-09-08 18:00</t>
+          <t>2021-10-07 18:00</t>
         </is>
       </c>
       <c r="B15" s="65" t="n">
-        <v>22</v>
-      </c>
-      <c r="C15" s="64" t="n">
-        <v>13</v>
-      </c>
-      <c r="D15" s="65" t="n">
-        <v>55</v>
+        <v>19</v>
+      </c>
+      <c r="C15" s="63" t="n">
+        <v>12</v>
+      </c>
+      <c r="D15" s="67" t="n">
+        <v>64</v>
       </c>
       <c r="E15" s="66" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F15" s="61" t="n">
-        <v>122</v>
-      </c>
-      <c r="G15" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
+        <v>299</v>
+      </c>
+      <c r="G15" s="72" t="inlineStr">
+        <is>
+          <t>9.6e-05</t>
         </is>
       </c>
       <c r="H15" s="66" t="inlineStr">
@@ -2593,46 +2527,46 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K15" s="66" t="inlineStr">
-        <is>
-          <t>4.3</t>
-        </is>
-      </c>
-      <c r="L15" s="66" t="inlineStr">
-        <is>
-          <t>1.5</t>
-        </is>
-      </c>
-      <c r="M15" s="66" t="inlineStr">
-        <is>
-          <t>3.5</t>
+      <c r="K15" s="73" t="inlineStr">
+        <is>
+          <t>68.7</t>
+        </is>
+      </c>
+      <c r="L15" s="61" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M15" s="61" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="61" t="inlineStr">
         <is>
-          <t>2021-09-08 21:00</t>
+          <t>2021-10-07 21:00</t>
         </is>
       </c>
       <c r="B16" s="65" t="n">
-        <v>21</v>
-      </c>
-      <c r="C16" s="63" t="n">
-        <v>12</v>
-      </c>
-      <c r="D16" s="65" t="n">
-        <v>55</v>
+        <v>18</v>
+      </c>
+      <c r="C16" s="64" t="n">
+        <v>13</v>
+      </c>
+      <c r="D16" s="67" t="n">
+        <v>70</v>
       </c>
       <c r="E16" s="66" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F16" s="61" t="n">
-        <v>50</v>
-      </c>
-      <c r="G16" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
+        <v>291</v>
+      </c>
+      <c r="G16" s="72" t="inlineStr">
+        <is>
+          <t>0.0001936</t>
         </is>
       </c>
       <c r="H16" s="66" t="inlineStr">
@@ -2650,42 +2584,42 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K16" s="70" t="inlineStr">
-        <is>
-          <t>11.2</t>
-        </is>
-      </c>
-      <c r="L16" s="66" t="inlineStr">
-        <is>
-          <t>2.9</t>
-        </is>
-      </c>
-      <c r="M16" s="71" t="inlineStr">
-        <is>
-          <t>5</t>
+      <c r="K16" s="68" t="inlineStr">
+        <is>
+          <t>36.3</t>
+        </is>
+      </c>
+      <c r="L16" s="70" t="inlineStr">
+        <is>
+          <t>16.9</t>
+        </is>
+      </c>
+      <c r="M16" s="70" t="inlineStr">
+        <is>
+          <t>10.8</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="61" t="inlineStr">
         <is>
-          <t>2021-09-09 00:00</t>
+          <t>2021-10-08 00:00</t>
         </is>
       </c>
       <c r="B17" s="65" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C17" s="63" t="n">
         <v>12</v>
       </c>
-      <c r="D17" s="65" t="n">
-        <v>56</v>
+      <c r="D17" s="69" t="n">
+        <v>77</v>
       </c>
       <c r="E17" s="66" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F17" s="61" t="n">
-        <v>61</v>
+        <v>219</v>
       </c>
       <c r="G17" s="66" t="inlineStr">
         <is>
@@ -2707,46 +2641,46 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K17" s="70" t="inlineStr">
-        <is>
-          <t>15.6</t>
-        </is>
-      </c>
-      <c r="L17" s="66" t="inlineStr">
-        <is>
-          <t>3.8</t>
-        </is>
-      </c>
-      <c r="M17" s="71" t="inlineStr">
-        <is>
-          <t>5.4</t>
+      <c r="K17" s="75" t="inlineStr">
+        <is>
+          <t>26.4</t>
+        </is>
+      </c>
+      <c r="L17" s="68" t="inlineStr">
+        <is>
+          <t>46.4</t>
+        </is>
+      </c>
+      <c r="M17" s="68" t="inlineStr">
+        <is>
+          <t>53.2</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="61" t="inlineStr">
         <is>
-          <t>2021-09-09 03:00</t>
+          <t>2021-10-08 03:00</t>
         </is>
       </c>
       <c r="B18" s="65" t="n">
-        <v>20</v>
-      </c>
-      <c r="C18" s="63" t="n">
-        <v>12</v>
-      </c>
-      <c r="D18" s="65" t="n">
-        <v>58</v>
+        <v>16</v>
+      </c>
+      <c r="C18" s="64" t="n">
+        <v>13</v>
+      </c>
+      <c r="D18" s="69" t="n">
+        <v>82</v>
       </c>
       <c r="E18" s="66" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F18" s="61" t="n">
-        <v>61</v>
-      </c>
-      <c r="G18" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
+        <v>313</v>
+      </c>
+      <c r="G18" s="72" t="inlineStr">
+        <is>
+          <t>0.0003312</t>
         </is>
       </c>
       <c r="H18" s="66" t="inlineStr">
@@ -2766,44 +2700,44 @@
       </c>
       <c r="K18" s="68" t="inlineStr">
         <is>
-          <t>47.8</t>
-        </is>
-      </c>
-      <c r="L18" s="70" t="inlineStr">
-        <is>
-          <t>20.6</t>
-        </is>
-      </c>
-      <c r="M18" s="68" t="inlineStr">
-        <is>
-          <t>44.8</t>
+          <t>37.3</t>
+        </is>
+      </c>
+      <c r="L18" s="68" t="inlineStr">
+        <is>
+          <t>42.9</t>
+        </is>
+      </c>
+      <c r="M18" s="61" t="inlineStr">
+        <is>
+          <t>83.1</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="61" t="inlineStr">
         <is>
-          <t>2021-09-09 06:00</t>
+          <t>2021-10-08 06:00</t>
         </is>
       </c>
       <c r="B19" s="65" t="n">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C19" s="64" t="n">
         <v>13</v>
       </c>
-      <c r="D19" s="65" t="n">
-        <v>55</v>
+      <c r="D19" s="69" t="n">
+        <v>74</v>
       </c>
       <c r="E19" s="66" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F19" s="61" t="n">
-        <v>133</v>
-      </c>
-      <c r="G19" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
+        <v>306</v>
+      </c>
+      <c r="G19" s="72" t="inlineStr">
+        <is>
+          <t>0.0001512</t>
         </is>
       </c>
       <c r="H19" s="66" t="inlineStr">
@@ -2823,40 +2757,40 @@
       </c>
       <c r="K19" s="68" t="inlineStr">
         <is>
-          <t>34.9</t>
+          <t>36.4</t>
         </is>
       </c>
       <c r="L19" s="68" t="inlineStr">
         <is>
-          <t>32.9</t>
-        </is>
-      </c>
-      <c r="M19" s="75" t="inlineStr">
-        <is>
-          <t>25.5</t>
+          <t>41.9</t>
+        </is>
+      </c>
+      <c r="M19" s="73" t="inlineStr">
+        <is>
+          <t>65.2</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="61" t="inlineStr">
         <is>
-          <t>2021-09-09 09:00</t>
-        </is>
-      </c>
-      <c r="B20" s="63" t="n">
-        <v>26</v>
+          <t>2021-10-08 09:00</t>
+        </is>
+      </c>
+      <c r="B20" s="65" t="n">
+        <v>20</v>
       </c>
       <c r="C20" s="63" t="n">
         <v>11</v>
       </c>
       <c r="D20" s="65" t="n">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="E20" s="66" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F20" s="61" t="n">
-        <v>47</v>
+        <v>268</v>
       </c>
       <c r="G20" s="66" t="inlineStr">
         <is>
@@ -2878,46 +2812,46 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K20" s="66" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="L20" s="71" t="inlineStr">
-        <is>
-          <t>5.3</t>
-        </is>
-      </c>
-      <c r="M20" s="71" t="inlineStr">
-        <is>
-          <t>6</t>
+      <c r="K20" s="71" t="inlineStr">
+        <is>
+          <t>9.4</t>
+        </is>
+      </c>
+      <c r="L20" s="70" t="inlineStr">
+        <is>
+          <t>10.8</t>
+        </is>
+      </c>
+      <c r="M20" s="68" t="inlineStr">
+        <is>
+          <t>52.6</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="61" t="inlineStr">
         <is>
-          <t>2021-09-09 12:00</t>
-        </is>
-      </c>
-      <c r="B21" s="63" t="n">
-        <v>27</v>
+          <t>2021-10-08 12:00</t>
+        </is>
+      </c>
+      <c r="B21" s="65" t="n">
+        <v>22</v>
       </c>
       <c r="C21" s="63" t="n">
         <v>11</v>
       </c>
       <c r="D21" s="65" t="n">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="E21" s="66" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F21" s="61" t="n">
-        <v>22</v>
-      </c>
-      <c r="G21" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
+        <v>234</v>
+      </c>
+      <c r="G21" s="72" t="inlineStr">
+        <is>
+          <t>1.92e-05</t>
         </is>
       </c>
       <c r="H21" s="66" t="inlineStr">
@@ -2935,46 +2869,46 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K21" s="71" t="inlineStr">
-        <is>
-          <t>6.3</t>
-        </is>
-      </c>
-      <c r="L21" s="71" t="inlineStr">
-        <is>
-          <t>6.1</t>
-        </is>
-      </c>
-      <c r="M21" s="66" t="inlineStr">
-        <is>
-          <t>4.2</t>
+      <c r="K21" s="70" t="inlineStr">
+        <is>
+          <t>12.4</t>
+        </is>
+      </c>
+      <c r="L21" s="75" t="inlineStr">
+        <is>
+          <t>26.9</t>
+        </is>
+      </c>
+      <c r="M21" s="73" t="inlineStr">
+        <is>
+          <t>60.1</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="61" t="inlineStr">
         <is>
-          <t>2021-09-09 15:00</t>
-        </is>
-      </c>
-      <c r="B22" s="63" t="n">
-        <v>24</v>
-      </c>
-      <c r="C22" s="64" t="n">
-        <v>13</v>
+          <t>2021-10-08 15:00</t>
+        </is>
+      </c>
+      <c r="B22" s="65" t="n">
+        <v>21</v>
+      </c>
+      <c r="C22" s="63" t="n">
+        <v>11</v>
       </c>
       <c r="D22" s="65" t="n">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="E22" s="66" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F22" s="61" t="n">
-        <v>205</v>
-      </c>
-      <c r="G22" s="72" t="inlineStr">
-        <is>
-          <t>6.48e-05</t>
+        <v>266</v>
+      </c>
+      <c r="G22" s="66" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="H22" s="66" t="inlineStr">
@@ -2994,44 +2928,44 @@
       </c>
       <c r="K22" s="75" t="inlineStr">
         <is>
-          <t>28.4</t>
-        </is>
-      </c>
-      <c r="L22" s="70" t="inlineStr">
-        <is>
-          <t>18.3</t>
-        </is>
-      </c>
-      <c r="M22" s="71" t="inlineStr">
-        <is>
-          <t>5.3</t>
+          <t>26.7</t>
+        </is>
+      </c>
+      <c r="L22" s="73" t="inlineStr">
+        <is>
+          <t>71.4</t>
+        </is>
+      </c>
+      <c r="M22" s="74" t="inlineStr">
+        <is>
+          <t>97.4</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="61" t="inlineStr">
         <is>
-          <t>2021-09-09 18:00</t>
+          <t>2021-10-08 18:00</t>
         </is>
       </c>
       <c r="B23" s="65" t="n">
-        <v>20</v>
-      </c>
-      <c r="C23" s="63" t="n">
-        <v>11</v>
-      </c>
-      <c r="D23" s="65" t="n">
-        <v>57</v>
+        <v>19</v>
+      </c>
+      <c r="C23" s="64" t="n">
+        <v>13</v>
+      </c>
+      <c r="D23" s="67" t="n">
+        <v>68</v>
       </c>
       <c r="E23" s="66" t="n">
         <v>2</v>
       </c>
       <c r="F23" s="61" t="n">
-        <v>177</v>
+        <v>255</v>
       </c>
       <c r="G23" s="72" t="inlineStr">
         <is>
-          <t>4.72e-05</t>
+          <t>1.04e-05</t>
         </is>
       </c>
       <c r="H23" s="66" t="inlineStr">
@@ -3049,46 +2983,46 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K23" s="75" t="inlineStr">
-        <is>
-          <t>23.5</t>
-        </is>
-      </c>
-      <c r="L23" s="70" t="inlineStr">
-        <is>
-          <t>18.6</t>
-        </is>
-      </c>
-      <c r="M23" s="68" t="inlineStr">
-        <is>
-          <t>40.8</t>
+      <c r="K23" s="70" t="inlineStr">
+        <is>
+          <t>19.4</t>
+        </is>
+      </c>
+      <c r="L23" s="73" t="inlineStr">
+        <is>
+          <t>70.2</t>
+        </is>
+      </c>
+      <c r="M23" s="61" t="inlineStr">
+        <is>
+          <t>85</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="61" t="inlineStr">
         <is>
-          <t>2021-09-09 21:00</t>
+          <t>2021-10-08 21:00</t>
         </is>
       </c>
       <c r="B24" s="65" t="n">
-        <v>21</v>
-      </c>
-      <c r="C24" s="63" t="n">
-        <v>11</v>
-      </c>
-      <c r="D24" s="65" t="n">
-        <v>55</v>
+        <v>18</v>
+      </c>
+      <c r="C24" s="64" t="n">
+        <v>13</v>
+      </c>
+      <c r="D24" s="69" t="n">
+        <v>76</v>
       </c>
       <c r="E24" s="66" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F24" s="61" t="n">
-        <v>281</v>
-      </c>
-      <c r="G24" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
+        <v>292</v>
+      </c>
+      <c r="G24" s="72" t="inlineStr">
+        <is>
+          <t>5.68e-05</t>
         </is>
       </c>
       <c r="H24" s="66" t="inlineStr">
@@ -3106,42 +3040,42 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K24" s="66" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="L24" s="70" t="inlineStr">
-        <is>
-          <t>18.1</t>
-        </is>
-      </c>
-      <c r="M24" s="68" t="inlineStr">
-        <is>
-          <t>42.2</t>
+      <c r="K24" s="70" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="L24" s="68" t="inlineStr">
+        <is>
+          <t>45.2</t>
+        </is>
+      </c>
+      <c r="M24" s="66" t="inlineStr">
+        <is>
+          <t>0.7</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="61" t="inlineStr">
         <is>
-          <t>2021-09-10 00:00</t>
+          <t>2021-10-09 00:00</t>
         </is>
       </c>
       <c r="B25" s="65" t="n">
-        <v>20</v>
-      </c>
-      <c r="C25" s="63" t="n">
-        <v>11</v>
-      </c>
-      <c r="D25" s="65" t="n">
-        <v>56</v>
+        <v>17</v>
+      </c>
+      <c r="C25" s="64" t="n">
+        <v>13</v>
+      </c>
+      <c r="D25" s="69" t="n">
+        <v>79</v>
       </c>
       <c r="E25" s="66" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F25" s="61" t="n">
-        <v>224</v>
+        <v>312</v>
       </c>
       <c r="G25" s="66" t="inlineStr">
         <is>
@@ -3165,44 +3099,44 @@
       </c>
       <c r="K25" s="71" t="inlineStr">
         <is>
-          <t>6.1</t>
+          <t>8.6</t>
         </is>
       </c>
       <c r="L25" s="75" t="inlineStr">
         <is>
-          <t>26.6</t>
-        </is>
-      </c>
-      <c r="M25" s="68" t="inlineStr">
-        <is>
-          <t>53</t>
+          <t>25.3</t>
+        </is>
+      </c>
+      <c r="M25" s="66" t="inlineStr">
+        <is>
+          <t>0.4</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="61" t="inlineStr">
         <is>
-          <t>2021-09-10 03:00</t>
+          <t>2021-10-09 03:00</t>
         </is>
       </c>
       <c r="B26" s="65" t="n">
-        <v>19</v>
-      </c>
-      <c r="C26" s="63" t="n">
-        <v>12</v>
-      </c>
-      <c r="D26" s="67" t="n">
-        <v>62</v>
+        <v>16</v>
+      </c>
+      <c r="C26" s="64" t="n">
+        <v>13</v>
+      </c>
+      <c r="D26" s="69" t="n">
+        <v>81</v>
       </c>
       <c r="E26" s="66" t="n">
         <v>1</v>
       </c>
       <c r="F26" s="61" t="n">
-        <v>245</v>
-      </c>
-      <c r="G26" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
+        <v>359</v>
+      </c>
+      <c r="G26" s="72" t="inlineStr">
+        <is>
+          <t>8e-07</t>
         </is>
       </c>
       <c r="H26" s="66" t="inlineStr">
@@ -3220,14 +3154,14 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K26" s="66" t="inlineStr">
-        <is>
-          <t>4.6</t>
-        </is>
-      </c>
-      <c r="L26" s="71" t="inlineStr">
-        <is>
-          <t>6.3</t>
+      <c r="K26" s="70" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="L26" s="75" t="inlineStr">
+        <is>
+          <t>22.9</t>
         </is>
       </c>
       <c r="M26" s="66" t="inlineStr">
@@ -3239,23 +3173,23 @@
     <row r="27">
       <c r="A27" s="61" t="inlineStr">
         <is>
-          <t>2021-09-10 06:00</t>
+          <t>2021-10-09 06:00</t>
         </is>
       </c>
       <c r="B27" s="65" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C27" s="64" t="n">
         <v>13</v>
       </c>
-      <c r="D27" s="65" t="n">
-        <v>59</v>
+      <c r="D27" s="69" t="n">
+        <v>73</v>
       </c>
       <c r="E27" s="66" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F27" s="61" t="n">
-        <v>247</v>
+        <v>25</v>
       </c>
       <c r="G27" s="66" t="inlineStr">
         <is>
@@ -3277,46 +3211,46 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K27" s="66" t="inlineStr">
-        <is>
-          <t>3.1</t>
-        </is>
-      </c>
-      <c r="L27" s="66" t="inlineStr">
-        <is>
-          <t>4.6</t>
+      <c r="K27" s="70" t="inlineStr">
+        <is>
+          <t>16.4</t>
+        </is>
+      </c>
+      <c r="L27" s="75" t="inlineStr">
+        <is>
+          <t>22.1</t>
         </is>
       </c>
       <c r="M27" s="66" t="inlineStr">
         <is>
-          <t>1.9</t>
+          <t>0.6</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="61" t="inlineStr">
         <is>
-          <t>2021-09-10 09:00</t>
-        </is>
-      </c>
-      <c r="B28" s="63" t="n">
-        <v>25</v>
-      </c>
-      <c r="C28" s="65" t="n">
-        <v>10</v>
+          <t>2021-10-09 09:00</t>
+        </is>
+      </c>
+      <c r="B28" s="65" t="n">
+        <v>21</v>
+      </c>
+      <c r="C28" s="64" t="n">
+        <v>13</v>
       </c>
       <c r="D28" s="65" t="n">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="E28" s="66" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F28" s="61" t="n">
-        <v>170</v>
-      </c>
-      <c r="G28" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
+        <v>13</v>
+      </c>
+      <c r="G28" s="72" t="inlineStr">
+        <is>
+          <t>8.8e-06</t>
         </is>
       </c>
       <c r="H28" s="66" t="inlineStr">
@@ -3334,46 +3268,46 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K28" s="66" t="inlineStr">
-        <is>
-          <t>4.2</t>
-        </is>
-      </c>
-      <c r="L28" s="61" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M28" s="66" t="inlineStr">
-        <is>
-          <t>0.4</t>
+      <c r="K28" s="75" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="L28" s="66" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="M28" s="61" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="61" t="inlineStr">
         <is>
-          <t>2021-09-10 12:00</t>
-        </is>
-      </c>
-      <c r="B29" s="63" t="n">
-        <v>28</v>
-      </c>
-      <c r="C29" s="65" t="n">
-        <v>9</v>
-      </c>
-      <c r="D29" s="63" t="n">
-        <v>30</v>
+          <t>2021-10-09 12:00</t>
+        </is>
+      </c>
+      <c r="B29" s="65" t="n">
+        <v>21</v>
+      </c>
+      <c r="C29" s="64" t="n">
+        <v>13</v>
+      </c>
+      <c r="D29" s="65" t="n">
+        <v>60</v>
       </c>
       <c r="E29" s="66" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F29" s="61" t="n">
-        <v>29</v>
-      </c>
-      <c r="G29" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
+        <v>14</v>
+      </c>
+      <c r="G29" s="72" t="inlineStr">
+        <is>
+          <t>0.0001224</t>
         </is>
       </c>
       <c r="H29" s="66" t="inlineStr">
@@ -3391,14 +3325,14 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K29" s="66" t="inlineStr">
-        <is>
-          <t>2.1</t>
-        </is>
-      </c>
-      <c r="L29" s="61" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K29" s="68" t="inlineStr">
+        <is>
+          <t>39.7</t>
+        </is>
+      </c>
+      <c r="L29" s="71" t="inlineStr">
+        <is>
+          <t>5.2</t>
         </is>
       </c>
       <c r="M29" s="66" t="inlineStr">
@@ -3410,27 +3344,27 @@
     <row r="30">
       <c r="A30" s="61" t="inlineStr">
         <is>
-          <t>2021-09-10 15:00</t>
-        </is>
-      </c>
-      <c r="B30" s="63" t="n">
-        <v>27</v>
-      </c>
-      <c r="C30" s="63" t="n">
-        <v>11</v>
-      </c>
-      <c r="D30" s="65" t="n">
-        <v>35</v>
+          <t>2021-10-09 15:00</t>
+        </is>
+      </c>
+      <c r="B30" s="65" t="n">
+        <v>19</v>
+      </c>
+      <c r="C30" s="64" t="n">
+        <v>13</v>
+      </c>
+      <c r="D30" s="67" t="n">
+        <v>65</v>
       </c>
       <c r="E30" s="66" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F30" s="61" t="n">
-        <v>258</v>
-      </c>
-      <c r="G30" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
+        <v>38</v>
+      </c>
+      <c r="G30" s="72" t="inlineStr">
+        <is>
+          <t>2.48e-05</t>
         </is>
       </c>
       <c r="H30" s="66" t="inlineStr">
@@ -3448,42 +3382,42 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K30" s="61" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L30" s="61" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M30" s="66" t="inlineStr">
-        <is>
-          <t>3.2</t>
+      <c r="K30" s="74" t="inlineStr">
+        <is>
+          <t>97.4</t>
+        </is>
+      </c>
+      <c r="L30" s="66" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="M30" s="68" t="inlineStr">
+        <is>
+          <t>51.5</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="61" t="inlineStr">
         <is>
-          <t>2021-09-10 18:00</t>
-        </is>
-      </c>
-      <c r="B31" s="63" t="n">
-        <v>23</v>
+          <t>2021-10-09 18:00</t>
+        </is>
+      </c>
+      <c r="B31" s="65" t="n">
+        <v>18</v>
       </c>
       <c r="C31" s="64" t="n">
-        <v>14</v>
-      </c>
-      <c r="D31" s="65" t="n">
-        <v>54</v>
+        <v>13</v>
+      </c>
+      <c r="D31" s="69" t="n">
+        <v>73</v>
       </c>
       <c r="E31" s="66" t="n">
         <v>3</v>
       </c>
       <c r="F31" s="61" t="n">
-        <v>215</v>
+        <v>39</v>
       </c>
       <c r="G31" s="66" t="inlineStr">
         <is>
@@ -3505,51 +3439,51 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K31" s="61" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L31" s="61" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M31" s="70" t="inlineStr">
-        <is>
-          <t>19.9</t>
+      <c r="K31" s="73" t="inlineStr">
+        <is>
+          <t>66.4</t>
+        </is>
+      </c>
+      <c r="L31" s="71" t="inlineStr">
+        <is>
+          <t>5.5</t>
+        </is>
+      </c>
+      <c r="M31" s="73" t="inlineStr">
+        <is>
+          <t>75.2</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="61" t="inlineStr">
         <is>
-          <t>2021-09-10 21:00</t>
+          <t>2021-10-09 21:00</t>
         </is>
       </c>
       <c r="B32" s="65" t="n">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C32" s="64" t="n">
         <v>14</v>
       </c>
-      <c r="D32" s="65" t="n">
-        <v>60</v>
+      <c r="D32" s="69" t="n">
+        <v>81</v>
       </c>
       <c r="E32" s="66" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F32" s="61" t="n">
-        <v>213</v>
-      </c>
-      <c r="G32" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H32" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
+        <v>55</v>
+      </c>
+      <c r="G32" s="72" t="inlineStr">
+        <is>
+          <t>0.000128</t>
+        </is>
+      </c>
+      <c r="H32" s="65" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="I32" s="66" t="inlineStr">
@@ -3562,51 +3496,51 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K32" s="61" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L32" s="61" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K32" s="70" t="inlineStr">
+        <is>
+          <t>17.8</t>
+        </is>
+      </c>
+      <c r="L32" s="71" t="inlineStr">
+        <is>
+          <t>7</t>
         </is>
       </c>
       <c r="M32" s="74" t="inlineStr">
         <is>
-          <t>91.9</t>
+          <t>100</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="61" t="inlineStr">
         <is>
-          <t>2021-09-11 00:00</t>
+          <t>2021-10-10 00:00</t>
         </is>
       </c>
       <c r="B33" s="65" t="n">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C33" s="64" t="n">
-        <v>15</v>
-      </c>
-      <c r="D33" s="67" t="n">
-        <v>65</v>
+        <v>14</v>
+      </c>
+      <c r="D33" s="69" t="n">
+        <v>79</v>
       </c>
       <c r="E33" s="66" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F33" s="61" t="n">
-        <v>206</v>
-      </c>
-      <c r="G33" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H33" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
+        <v>55</v>
+      </c>
+      <c r="G33" s="72" t="inlineStr">
+        <is>
+          <t>0.0001776</t>
+        </is>
+      </c>
+      <c r="H33" s="65" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="I33" s="66" t="inlineStr">
@@ -3619,51 +3553,51 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K33" s="61" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L33" s="61" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K33" s="68" t="inlineStr">
+        <is>
+          <t>52.6</t>
+        </is>
+      </c>
+      <c r="L33" s="70" t="inlineStr">
+        <is>
+          <t>17.6</t>
         </is>
       </c>
       <c r="M33" s="74" t="inlineStr">
         <is>
-          <t>95.6</t>
+          <t>98.7</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="61" t="inlineStr">
         <is>
-          <t>2021-09-11 03:00</t>
+          <t>2021-10-10 03:00</t>
         </is>
       </c>
       <c r="B34" s="65" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C34" s="64" t="n">
-        <v>15</v>
-      </c>
-      <c r="D34" s="67" t="n">
-        <v>67</v>
+        <v>14</v>
+      </c>
+      <c r="D34" s="69" t="n">
+        <v>83</v>
       </c>
       <c r="E34" s="66" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F34" s="61" t="n">
-        <v>5</v>
-      </c>
-      <c r="G34" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H34" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
+        <v>32</v>
+      </c>
+      <c r="G34" s="72" t="inlineStr">
+        <is>
+          <t>0.000164</t>
+        </is>
+      </c>
+      <c r="H34" s="65" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="I34" s="66" t="inlineStr">
@@ -3676,51 +3610,51 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K34" s="61" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L34" s="61" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M34" s="74" t="inlineStr">
-        <is>
-          <t>99.5</t>
+      <c r="K34" s="74" t="inlineStr">
+        <is>
+          <t>99.7</t>
+        </is>
+      </c>
+      <c r="L34" s="71" t="inlineStr">
+        <is>
+          <t>7.6</t>
+        </is>
+      </c>
+      <c r="M34" s="71" t="inlineStr">
+        <is>
+          <t>5.7</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="61" t="inlineStr">
         <is>
-          <t>2021-09-11 06:00</t>
-        </is>
-      </c>
-      <c r="B35" s="63" t="n">
-        <v>23</v>
+          <t>2021-10-10 06:00</t>
+        </is>
+      </c>
+      <c r="B35" s="65" t="n">
+        <v>16</v>
       </c>
       <c r="C35" s="64" t="n">
         <v>15</v>
       </c>
-      <c r="D35" s="65" t="n">
-        <v>60</v>
+      <c r="D35" s="69" t="n">
+        <v>92</v>
       </c>
       <c r="E35" s="66" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F35" s="61" t="n">
-        <v>305</v>
+        <v>334</v>
       </c>
       <c r="G35" s="72" t="inlineStr">
         <is>
-          <t>1.08e-05</t>
-        </is>
-      </c>
-      <c r="H35" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
+          <t>0.0027376</t>
+        </is>
+      </c>
+      <c r="H35" s="65" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="I35" s="66" t="inlineStr">
@@ -3733,51 +3667,51 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K35" s="61" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L35" s="66" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="M35" s="73" t="inlineStr">
-        <is>
-          <t>66</t>
+      <c r="K35" s="74" t="inlineStr">
+        <is>
+          <t>99.8</t>
+        </is>
+      </c>
+      <c r="L35" s="70" t="inlineStr">
+        <is>
+          <t>21.1</t>
+        </is>
+      </c>
+      <c r="M35" s="66" t="inlineStr">
+        <is>
+          <t>4.5</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="61" t="inlineStr">
         <is>
-          <t>2021-09-11 09:00</t>
-        </is>
-      </c>
-      <c r="B36" s="63" t="n">
-        <v>26</v>
-      </c>
-      <c r="C36" s="63" t="n">
-        <v>12</v>
-      </c>
-      <c r="D36" s="65" t="n">
-        <v>39</v>
+          <t>2021-10-10 09:00</t>
+        </is>
+      </c>
+      <c r="B36" s="65" t="n">
+        <v>18</v>
+      </c>
+      <c r="C36" s="64" t="n">
+        <v>14</v>
+      </c>
+      <c r="D36" s="69" t="n">
+        <v>82</v>
       </c>
       <c r="E36" s="66" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F36" s="61" t="n">
-        <v>254</v>
-      </c>
-      <c r="G36" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H36" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
+        <v>346</v>
+      </c>
+      <c r="G36" s="72" t="inlineStr">
+        <is>
+          <t>0.0008924</t>
+        </is>
+      </c>
+      <c r="H36" s="65" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="I36" s="66" t="inlineStr">
@@ -3790,51 +3724,51 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K36" s="61" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L36" s="71" t="inlineStr">
-        <is>
-          <t>6.1</t>
-        </is>
-      </c>
-      <c r="M36" s="68" t="inlineStr">
-        <is>
-          <t>34</t>
+      <c r="K36" s="74" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="L36" s="74" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="M36" s="74" t="inlineStr">
+        <is>
+          <t>99.9</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="61" t="inlineStr">
         <is>
-          <t>2021-09-11 12:00</t>
-        </is>
-      </c>
-      <c r="B37" s="63" t="n">
-        <v>28</v>
-      </c>
-      <c r="C37" s="63" t="n">
-        <v>11</v>
-      </c>
-      <c r="D37" s="65" t="n">
-        <v>36</v>
+          <t>2021-10-10 12:00</t>
+        </is>
+      </c>
+      <c r="B37" s="65" t="n">
+        <v>19</v>
+      </c>
+      <c r="C37" s="64" t="n">
+        <v>15</v>
+      </c>
+      <c r="D37" s="69" t="n">
+        <v>77</v>
       </c>
       <c r="E37" s="66" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F37" s="61" t="n">
-        <v>211</v>
-      </c>
-      <c r="G37" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H37" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
+        <v>333</v>
+      </c>
+      <c r="G37" s="72" t="inlineStr">
+        <is>
+          <t>0.000398</t>
+        </is>
+      </c>
+      <c r="H37" s="65" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="I37" s="66" t="inlineStr">
@@ -3847,51 +3781,51 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K37" s="61" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L37" s="75" t="inlineStr">
-        <is>
-          <t>29.8</t>
-        </is>
-      </c>
-      <c r="M37" s="68" t="inlineStr">
-        <is>
-          <t>45.5</t>
+      <c r="K37" s="74" t="inlineStr">
+        <is>
+          <t>94.6</t>
+        </is>
+      </c>
+      <c r="L37" s="73" t="inlineStr">
+        <is>
+          <t>69.6</t>
+        </is>
+      </c>
+      <c r="M37" s="61" t="inlineStr">
+        <is>
+          <t>80.8</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="61" t="inlineStr">
         <is>
-          <t>2021-09-11 15:00</t>
-        </is>
-      </c>
-      <c r="B38" s="63" t="n">
-        <v>24</v>
+          <t>2021-10-10 15:00</t>
+        </is>
+      </c>
+      <c r="B38" s="65" t="n">
+        <v>19</v>
       </c>
       <c r="C38" s="64" t="n">
-        <v>14</v>
-      </c>
-      <c r="D38" s="65" t="n">
-        <v>52</v>
+        <v>15</v>
+      </c>
+      <c r="D38" s="69" t="n">
+        <v>80</v>
       </c>
       <c r="E38" s="66" t="n">
         <v>6</v>
       </c>
       <c r="F38" s="61" t="n">
-        <v>206</v>
-      </c>
-      <c r="G38" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H38" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
+        <v>314</v>
+      </c>
+      <c r="G38" s="72" t="inlineStr">
+        <is>
+          <t>0.0009128</t>
+        </is>
+      </c>
+      <c r="H38" s="65" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="I38" s="66" t="inlineStr">
@@ -3906,12 +3840,12 @@
       </c>
       <c r="K38" s="68" t="inlineStr">
         <is>
-          <t>48.6</t>
-        </is>
-      </c>
-      <c r="L38" s="74" t="inlineStr">
-        <is>
-          <t>96.4</t>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="L38" s="71" t="inlineStr">
+        <is>
+          <t>7</t>
         </is>
       </c>
       <c r="M38" s="74" t="inlineStr">
@@ -3923,32 +3857,32 @@
     <row r="39">
       <c r="A39" s="61" t="inlineStr">
         <is>
-          <t>2021-09-11 18:00</t>
+          <t>2021-10-10 18:00</t>
         </is>
       </c>
       <c r="B39" s="65" t="n">
-        <v>21</v>
-      </c>
-      <c r="C39" s="63" t="n">
-        <v>11</v>
-      </c>
-      <c r="D39" s="65" t="n">
-        <v>53</v>
+        <v>18</v>
+      </c>
+      <c r="C39" s="64" t="n">
+        <v>15</v>
+      </c>
+      <c r="D39" s="69" t="n">
+        <v>86</v>
       </c>
       <c r="E39" s="66" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F39" s="61" t="n">
-        <v>213</v>
-      </c>
-      <c r="G39" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H39" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
+        <v>333</v>
+      </c>
+      <c r="G39" s="72" t="inlineStr">
+        <is>
+          <t>0.0008776</t>
+        </is>
+      </c>
+      <c r="H39" s="65" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="I39" s="66" t="inlineStr">
@@ -3961,14 +3895,14 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K39" s="75" t="inlineStr">
-        <is>
-          <t>28.9</t>
-        </is>
-      </c>
-      <c r="L39" s="74" t="inlineStr">
-        <is>
-          <t>98.2</t>
+      <c r="K39" s="68" t="inlineStr">
+        <is>
+          <t>55.9</t>
+        </is>
+      </c>
+      <c r="L39" s="68" t="inlineStr">
+        <is>
+          <t>47</t>
         </is>
       </c>
       <c r="M39" s="74" t="inlineStr">
@@ -3980,32 +3914,32 @@
     <row r="40">
       <c r="A40" s="61" t="inlineStr">
         <is>
-          <t>2021-09-11 21:00</t>
+          <t>2021-10-10 21:00</t>
         </is>
       </c>
       <c r="B40" s="65" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C40" s="64" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D40" s="69" t="n">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="E40" s="66" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F40" s="61" t="n">
-        <v>213</v>
+        <v>332</v>
       </c>
       <c r="G40" s="72" t="inlineStr">
         <is>
-          <t>9.6e-06</t>
-        </is>
-      </c>
-      <c r="H40" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
+          <t>0.0012064</t>
+        </is>
+      </c>
+      <c r="H40" s="65" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="I40" s="66" t="inlineStr">
@@ -4018,51 +3952,51 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K40" s="71" t="inlineStr">
-        <is>
-          <t>5.9</t>
+      <c r="K40" s="74" t="inlineStr">
+        <is>
+          <t>95.3</t>
         </is>
       </c>
       <c r="L40" s="74" t="inlineStr">
         <is>
-          <t>93</t>
-        </is>
-      </c>
-      <c r="M40" s="73" t="inlineStr">
-        <is>
-          <t>70.2</t>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="M40" s="74" t="inlineStr">
+        <is>
+          <t>100</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="61" t="inlineStr">
         <is>
-          <t>2021-09-12 00:00</t>
+          <t>2021-10-11 00:00</t>
         </is>
       </c>
       <c r="B41" s="65" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C41" s="64" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D41" s="69" t="n">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="E41" s="66" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F41" s="61" t="n">
-        <v>184</v>
-      </c>
-      <c r="G41" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H41" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
+        <v>334</v>
+      </c>
+      <c r="G41" s="72" t="inlineStr">
+        <is>
+          <t>0.001592</t>
+        </is>
+      </c>
+      <c r="H41" s="65" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="I41" s="66" t="inlineStr">
@@ -4075,51 +4009,51 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K41" s="70" t="inlineStr">
-        <is>
-          <t>12.4</t>
-        </is>
-      </c>
-      <c r="L41" s="68" t="inlineStr">
-        <is>
-          <t>52.3</t>
-        </is>
-      </c>
-      <c r="M41" s="68" t="inlineStr">
-        <is>
-          <t>42.9</t>
+      <c r="K41" s="74" t="inlineStr">
+        <is>
+          <t>97.6</t>
+        </is>
+      </c>
+      <c r="L41" s="74" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="M41" s="74" t="inlineStr">
+        <is>
+          <t>100</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="61" t="inlineStr">
         <is>
-          <t>2021-09-12 03:00</t>
+          <t>2021-10-11 03:00</t>
         </is>
       </c>
       <c r="B42" s="65" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C42" s="64" t="n">
-        <v>14</v>
-      </c>
-      <c r="D42" s="67" t="n">
-        <v>67</v>
+        <v>15</v>
+      </c>
+      <c r="D42" s="69" t="n">
+        <v>82</v>
       </c>
       <c r="E42" s="66" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F42" s="61" t="n">
-        <v>199</v>
-      </c>
-      <c r="G42" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H42" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
+        <v>307</v>
+      </c>
+      <c r="G42" s="72" t="inlineStr">
+        <is>
+          <t>0.0009364</t>
+        </is>
+      </c>
+      <c r="H42" s="65" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="I42" s="66" t="inlineStr">
@@ -4132,51 +4066,51 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K42" s="74" t="inlineStr">
-        <is>
-          <t>97.6</t>
-        </is>
-      </c>
-      <c r="L42" s="70" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="M42" s="73" t="inlineStr">
-        <is>
-          <t>68.2</t>
+      <c r="K42" s="68" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="L42" s="74" t="inlineStr">
+        <is>
+          <t>99.3</t>
+        </is>
+      </c>
+      <c r="M42" s="74" t="inlineStr">
+        <is>
+          <t>100</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="61" t="inlineStr">
         <is>
-          <t>2021-09-12 06:00</t>
+          <t>2021-10-11 06:00</t>
         </is>
       </c>
       <c r="B43" s="65" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C43" s="64" t="n">
-        <v>13</v>
-      </c>
-      <c r="D43" s="67" t="n">
-        <v>65</v>
+        <v>15</v>
+      </c>
+      <c r="D43" s="69" t="n">
+        <v>83</v>
       </c>
       <c r="E43" s="66" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F43" s="61" t="n">
-        <v>353</v>
-      </c>
-      <c r="G43" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H43" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
+        <v>321</v>
+      </c>
+      <c r="G43" s="72" t="inlineStr">
+        <is>
+          <t>0.0008128</t>
+        </is>
+      </c>
+      <c r="H43" s="65" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="I43" s="66" t="inlineStr">
@@ -4189,51 +4123,51 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K43" s="74" t="inlineStr">
-        <is>
-          <t>98.8</t>
-        </is>
-      </c>
-      <c r="L43" s="68" t="inlineStr">
-        <is>
-          <t>46.1</t>
-        </is>
-      </c>
-      <c r="M43" s="73" t="inlineStr">
-        <is>
-          <t>64.3</t>
+      <c r="K43" s="68" t="inlineStr">
+        <is>
+          <t>50.8</t>
+        </is>
+      </c>
+      <c r="L43" s="74" t="inlineStr">
+        <is>
+          <t>99.4</t>
+        </is>
+      </c>
+      <c r="M43" s="74" t="inlineStr">
+        <is>
+          <t>100</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="61" t="inlineStr">
         <is>
-          <t>2021-09-12 09:00</t>
+          <t>2021-10-11 09:00</t>
         </is>
       </c>
       <c r="B44" s="65" t="n">
-        <v>22</v>
-      </c>
-      <c r="C44" s="63" t="n">
-        <v>12</v>
-      </c>
-      <c r="D44" s="65" t="n">
-        <v>55</v>
+        <v>18</v>
+      </c>
+      <c r="C44" s="64" t="n">
+        <v>15</v>
+      </c>
+      <c r="D44" s="69" t="n">
+        <v>82</v>
       </c>
       <c r="E44" s="66" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F44" s="61" t="n">
-        <v>247</v>
-      </c>
-      <c r="G44" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H44" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
+        <v>319</v>
+      </c>
+      <c r="G44" s="72" t="inlineStr">
+        <is>
+          <t>0.0004496</t>
+        </is>
+      </c>
+      <c r="H44" s="65" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="I44" s="66" t="inlineStr">
@@ -4246,51 +4180,51 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K44" s="74" t="inlineStr">
-        <is>
-          <t>97.8</t>
+      <c r="K44" s="73" t="inlineStr">
+        <is>
+          <t>68.2</t>
         </is>
       </c>
       <c r="L44" s="74" t="inlineStr">
         <is>
-          <t>91.7</t>
-        </is>
-      </c>
-      <c r="M44" s="70" t="inlineStr">
-        <is>
-          <t>11.6</t>
+          <t>93.2</t>
+        </is>
+      </c>
+      <c r="M44" s="74" t="inlineStr">
+        <is>
+          <t>100</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="61" t="inlineStr">
         <is>
-          <t>2021-09-12 12:00</t>
+          <t>2021-10-11 12:00</t>
         </is>
       </c>
       <c r="B45" s="65" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C45" s="64" t="n">
-        <v>13</v>
-      </c>
-      <c r="D45" s="65" t="n">
-        <v>57</v>
+        <v>15</v>
+      </c>
+      <c r="D45" s="69" t="n">
+        <v>82</v>
       </c>
       <c r="E45" s="66" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F45" s="61" t="n">
-        <v>143</v>
-      </c>
-      <c r="G45" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H45" s="66" t="inlineStr">
-        <is>
-          <t>0</t>
+        <v>324</v>
+      </c>
+      <c r="G45" s="72" t="inlineStr">
+        <is>
+          <t>0.000524</t>
+        </is>
+      </c>
+      <c r="H45" s="65" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="I45" s="66" t="inlineStr">
@@ -4305,22 +4239,22 @@
       </c>
       <c r="K45" s="74" t="inlineStr">
         <is>
-          <t>98.7</t>
+          <t>81.6</t>
         </is>
       </c>
       <c r="L45" s="74" t="inlineStr">
         <is>
-          <t>95.9</t>
-        </is>
-      </c>
-      <c r="M45" s="70" t="inlineStr">
-        <is>
-          <t>10.3</t>
+          <t>96.6</t>
+        </is>
+      </c>
+      <c r="M45" s="74" t="inlineStr">
+        <is>
+          <t>100</t>
         </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Improved Snow line graph
</commit_message>
<xml_diff>
--- a/simpleWeather.xlsx
+++ b/simpleWeather.xlsx
@@ -1840,7 +1840,7 @@
     <row r="2">
       <c r="A2" s="77" t="inlineStr">
         <is>
-          <t>2021-12-01 15:00 mer</t>
+          <t xml:space="preserve">2021-12-01 15:00 mer </t>
         </is>
       </c>
       <c r="B2" s="83" t="n">
@@ -1897,7 +1897,7 @@
     <row r="3">
       <c r="A3" s="77" t="inlineStr">
         <is>
-          <t>2021-12-01 18:00 mer</t>
+          <t xml:space="preserve">2021-12-01 18:00 mer </t>
         </is>
       </c>
       <c r="B3" s="83" t="n">
@@ -1954,7 +1954,7 @@
     <row r="4">
       <c r="A4" s="77" t="inlineStr">
         <is>
-          <t>2021-12-01 21:00 mer</t>
+          <t xml:space="preserve">2021-12-01 21:00 mer </t>
         </is>
       </c>
       <c r="B4" s="83" t="n">
@@ -2011,7 +2011,7 @@
     <row r="5">
       <c r="A5" s="77" t="inlineStr">
         <is>
-          <t>2021-12-02 00:00 gio</t>
+          <t xml:space="preserve">2021-12-02 00:00 gio </t>
         </is>
       </c>
       <c r="B5" s="83" t="n">
@@ -2068,7 +2068,7 @@
     <row r="6">
       <c r="A6" s="77" t="inlineStr">
         <is>
-          <t>2021-12-02 03:00 gio</t>
+          <t xml:space="preserve">2021-12-02 03:00 gio </t>
         </is>
       </c>
       <c r="B6" s="83" t="n">
@@ -2125,7 +2125,7 @@
     <row r="7">
       <c r="A7" s="77" t="inlineStr">
         <is>
-          <t>2021-12-02 06:00 gio</t>
+          <t xml:space="preserve">2021-12-02 06:00 gio </t>
         </is>
       </c>
       <c r="B7" s="83" t="n">
@@ -2182,7 +2182,7 @@
     <row r="8">
       <c r="A8" s="77" t="inlineStr">
         <is>
-          <t>2021-12-02 09:00 gio</t>
+          <t xml:space="preserve">2021-12-02 09:00 gio </t>
         </is>
       </c>
       <c r="B8" s="81" t="n">
@@ -2239,7 +2239,7 @@
     <row r="9">
       <c r="A9" s="77" t="inlineStr">
         <is>
-          <t>2021-12-02 12:00 gio</t>
+          <t xml:space="preserve">2021-12-02 12:00 gio </t>
         </is>
       </c>
       <c r="B9" s="81" t="n">
@@ -2296,7 +2296,7 @@
     <row r="10">
       <c r="A10" s="77" t="inlineStr">
         <is>
-          <t>2021-12-02 15:00 gio</t>
+          <t xml:space="preserve">2021-12-02 15:00 gio </t>
         </is>
       </c>
       <c r="B10" s="81" t="n">
@@ -2353,7 +2353,7 @@
     <row r="11">
       <c r="A11" s="77" t="inlineStr">
         <is>
-          <t>2021-12-02 18:00 gio</t>
+          <t xml:space="preserve">2021-12-02 18:00 gio </t>
         </is>
       </c>
       <c r="B11" s="81" t="n">
@@ -2410,7 +2410,7 @@
     <row r="12">
       <c r="A12" s="77" t="inlineStr">
         <is>
-          <t>2021-12-02 21:00 gio</t>
+          <t xml:space="preserve">2021-12-02 21:00 gio </t>
         </is>
       </c>
       <c r="B12" s="81" t="n">
@@ -2467,7 +2467,7 @@
     <row r="13">
       <c r="A13" s="77" t="inlineStr">
         <is>
-          <t>2021-12-03 00:00 ven</t>
+          <t xml:space="preserve">2021-12-03 00:00 ven </t>
         </is>
       </c>
       <c r="B13" s="81" t="n">
@@ -2524,7 +2524,7 @@
     <row r="14">
       <c r="A14" s="77" t="inlineStr">
         <is>
-          <t>2021-12-03 03:00 ven</t>
+          <t xml:space="preserve">2021-12-03 03:00 ven </t>
         </is>
       </c>
       <c r="B14" s="81" t="n">
@@ -2581,7 +2581,7 @@
     <row r="15">
       <c r="A15" s="77" t="inlineStr">
         <is>
-          <t>2021-12-03 06:00 ven</t>
+          <t xml:space="preserve">2021-12-03 06:00 ven </t>
         </is>
       </c>
       <c r="B15" s="81" t="n">
@@ -2638,7 +2638,7 @@
     <row r="16">
       <c r="A16" s="77" t="inlineStr">
         <is>
-          <t>2021-12-03 09:00 ven</t>
+          <t xml:space="preserve">2021-12-03 09:00 ven </t>
         </is>
       </c>
       <c r="B16" s="81" t="n">
@@ -2695,7 +2695,7 @@
     <row r="17">
       <c r="A17" s="77" t="inlineStr">
         <is>
-          <t>2021-12-03 12:00 ven</t>
+          <t xml:space="preserve">2021-12-03 12:00 ven </t>
         </is>
       </c>
       <c r="B17" s="81" t="n">
@@ -2752,7 +2752,7 @@
     <row r="18">
       <c r="A18" s="77" t="inlineStr">
         <is>
-          <t>2021-12-03 15:00 ven</t>
+          <t xml:space="preserve">2021-12-03 15:00 ven </t>
         </is>
       </c>
       <c r="B18" s="81" t="n">
@@ -2809,7 +2809,7 @@
     <row r="19">
       <c r="A19" s="77" t="inlineStr">
         <is>
-          <t>2021-12-03 18:00 ven</t>
+          <t xml:space="preserve">2021-12-03 18:00 ven </t>
         </is>
       </c>
       <c r="B19" s="91" t="n">
@@ -2866,7 +2866,7 @@
     <row r="20">
       <c r="A20" s="77" t="inlineStr">
         <is>
-          <t>2021-12-03 21:00 ven</t>
+          <t xml:space="preserve">2021-12-03 21:00 ven </t>
         </is>
       </c>
       <c r="B20" s="91" t="n">
@@ -2923,7 +2923,7 @@
     <row r="21">
       <c r="A21" s="77" t="inlineStr">
         <is>
-          <t>2021-12-04 00:00 sab</t>
+          <t xml:space="preserve">2021-12-04 00:00 sab </t>
         </is>
       </c>
       <c r="B21" s="91" t="n">
@@ -2980,7 +2980,7 @@
     <row r="22">
       <c r="A22" s="77" t="inlineStr">
         <is>
-          <t>2021-12-04 03:00 sab</t>
+          <t xml:space="preserve">2021-12-04 03:00 sab </t>
         </is>
       </c>
       <c r="B22" s="91" t="n">
@@ -3037,7 +3037,7 @@
     <row r="23">
       <c r="A23" s="77" t="inlineStr">
         <is>
-          <t>2021-12-04 06:00 sab</t>
+          <t xml:space="preserve">2021-12-04 06:00 sab </t>
         </is>
       </c>
       <c r="B23" s="83" t="n">
@@ -3094,7 +3094,7 @@
     <row r="24">
       <c r="A24" s="77" t="inlineStr">
         <is>
-          <t>2021-12-04 09:00 sab</t>
+          <t xml:space="preserve">2021-12-04 09:00 sab </t>
         </is>
       </c>
       <c r="B24" s="91" t="n">
@@ -3151,7 +3151,7 @@
     <row r="25">
       <c r="A25" s="77" t="inlineStr">
         <is>
-          <t>2021-12-04 12:00 sab</t>
+          <t xml:space="preserve">2021-12-04 12:00 sab </t>
         </is>
       </c>
       <c r="B25" s="91" t="n">
@@ -3208,7 +3208,7 @@
     <row r="26">
       <c r="A26" s="77" t="inlineStr">
         <is>
-          <t>2021-12-04 15:00 sab</t>
+          <t xml:space="preserve">2021-12-04 15:00 sab </t>
         </is>
       </c>
       <c r="B26" s="91" t="n">
@@ -3265,7 +3265,7 @@
     <row r="27">
       <c r="A27" s="77" t="inlineStr">
         <is>
-          <t>2021-12-04 18:00 sab</t>
+          <t xml:space="preserve">2021-12-04 18:00 sab </t>
         </is>
       </c>
       <c r="B27" s="83" t="n">
@@ -3322,7 +3322,7 @@
     <row r="28">
       <c r="A28" s="77" t="inlineStr">
         <is>
-          <t>2021-12-04 21:00 sab</t>
+          <t xml:space="preserve">2021-12-04 21:00 sab </t>
         </is>
       </c>
       <c r="B28" s="83" t="n">
@@ -3379,7 +3379,7 @@
     <row r="29">
       <c r="A29" s="77" t="inlineStr">
         <is>
-          <t>2021-12-05 00:00 dom</t>
+          <t xml:space="preserve">2021-12-05 00:00 dom </t>
         </is>
       </c>
       <c r="B29" s="83" t="n">
@@ -3436,7 +3436,7 @@
     <row r="30">
       <c r="A30" s="77" t="inlineStr">
         <is>
-          <t>2021-12-05 03:00 dom</t>
+          <t xml:space="preserve">2021-12-05 03:00 dom </t>
         </is>
       </c>
       <c r="B30" s="83" t="n">
@@ -3493,7 +3493,7 @@
     <row r="31">
       <c r="A31" s="77" t="inlineStr">
         <is>
-          <t>2021-12-05 06:00 dom</t>
+          <t xml:space="preserve">2021-12-05 06:00 dom </t>
         </is>
       </c>
       <c r="B31" s="83" t="n">
@@ -3550,7 +3550,7 @@
     <row r="32">
       <c r="A32" s="77" t="inlineStr">
         <is>
-          <t>2021-12-05 09:00 dom</t>
+          <t xml:space="preserve">2021-12-05 09:00 dom </t>
         </is>
       </c>
       <c r="B32" s="81" t="n">
@@ -3607,7 +3607,7 @@
     <row r="33">
       <c r="A33" s="77" t="inlineStr">
         <is>
-          <t>2021-12-05 12:00 dom</t>
+          <t xml:space="preserve">2021-12-05 12:00 dom </t>
         </is>
       </c>
       <c r="B33" s="81" t="n">
@@ -3664,7 +3664,7 @@
     <row r="34">
       <c r="A34" s="77" t="inlineStr">
         <is>
-          <t>2021-12-05 15:00 dom</t>
+          <t xml:space="preserve">2021-12-05 15:00 dom </t>
         </is>
       </c>
       <c r="B34" s="81" t="n">
@@ -3721,7 +3721,7 @@
     <row r="35">
       <c r="A35" s="77" t="inlineStr">
         <is>
-          <t>2021-12-05 18:00 dom</t>
+          <t xml:space="preserve">2021-12-05 18:00 dom </t>
         </is>
       </c>
       <c r="B35" s="91" t="n">
@@ -3778,7 +3778,7 @@
     <row r="36">
       <c r="A36" s="77" t="inlineStr">
         <is>
-          <t>2021-12-05 21:00 dom</t>
+          <t xml:space="preserve">2021-12-05 21:00 dom </t>
         </is>
       </c>
       <c r="B36" s="91" t="n">
@@ -3835,7 +3835,7 @@
     <row r="37">
       <c r="A37" s="77" t="inlineStr">
         <is>
-          <t>2021-12-06 00:00 lun</t>
+          <t xml:space="preserve">2021-12-06 00:00 lun </t>
         </is>
       </c>
       <c r="B37" s="83" t="n">
@@ -3892,7 +3892,7 @@
     <row r="38">
       <c r="A38" s="77" t="inlineStr">
         <is>
-          <t>2021-12-06 03:00 lun</t>
+          <t xml:space="preserve">2021-12-06 03:00 lun </t>
         </is>
       </c>
       <c r="B38" s="83" t="n">
@@ -3949,7 +3949,7 @@
     <row r="39">
       <c r="A39" s="77" t="inlineStr">
         <is>
-          <t>2021-12-06 06:00 lun</t>
+          <t xml:space="preserve">2021-12-06 06:00 lun </t>
         </is>
       </c>
       <c r="B39" s="83" t="n">
@@ -4006,7 +4006,7 @@
     <row r="40">
       <c r="A40" s="77" t="inlineStr">
         <is>
-          <t>2021-12-06 09:00 lun</t>
+          <t xml:space="preserve">2021-12-06 09:00 lun </t>
         </is>
       </c>
       <c r="B40" s="91" t="n">
@@ -4063,7 +4063,7 @@
     <row r="41">
       <c r="A41" s="77" t="inlineStr">
         <is>
-          <t>2021-12-06 12:00 lun</t>
+          <t xml:space="preserve">2021-12-06 12:00 lun </t>
         </is>
       </c>
       <c r="B41" s="91" t="n">
@@ -4120,7 +4120,7 @@
     <row r="42">
       <c r="A42" s="77" t="inlineStr">
         <is>
-          <t>2021-12-06 15:00 lun</t>
+          <t xml:space="preserve">2021-12-06 15:00 lun </t>
         </is>
       </c>
       <c r="B42" s="83" t="n">
@@ -4177,7 +4177,7 @@
     <row r="43">
       <c r="A43" s="77" t="inlineStr">
         <is>
-          <t>2021-12-06 18:00 lun</t>
+          <t xml:space="preserve">2021-12-06 18:00 lun </t>
         </is>
       </c>
       <c r="B43" s="83" t="n">
@@ -4234,7 +4234,7 @@
     <row r="44">
       <c r="A44" s="77" t="inlineStr">
         <is>
-          <t>2021-12-06 21:00 lun</t>
+          <t xml:space="preserve">2021-12-06 21:00 lun </t>
         </is>
       </c>
       <c r="B44" s="83" t="n">
@@ -4291,7 +4291,7 @@
     <row r="45">
       <c r="A45" s="77" t="inlineStr">
         <is>
-          <t>2021-12-07 00:00 mar</t>
+          <t xml:space="preserve">2021-12-07 00:00 mar </t>
         </is>
       </c>
       <c r="B45" s="83" t="n">

</xml_diff>

<commit_message>
Added 'DATA' on the first cell in xlsx simple weather
</commit_message>
<xml_diff>
--- a/simpleWeather.xlsx
+++ b/simpleWeather.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Foglio1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Foglio1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="162913" fullCalcOnLoad="1"/>
@@ -224,6 +224,7 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -344,79 +345,11 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>5</col>
@@ -431,13 +364,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -456,13 +389,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -481,13 +414,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId3"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId3"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -506,13 +439,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId4"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId4"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -531,13 +464,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId5"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId5"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -556,13 +489,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId6"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId6"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -581,13 +514,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId7"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId7"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -606,13 +539,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId8"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId8"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -631,13 +564,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId9"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId9"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -656,13 +589,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId10"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId10"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -681,13 +614,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId11"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId11"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -706,13 +639,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId12"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId12"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -731,13 +664,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId13"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId13"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -756,13 +689,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId14"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId14"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -781,13 +714,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId15"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId15"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -806,13 +739,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId16"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId16"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -831,13 +764,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId17"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId17"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -856,13 +789,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId18"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId18"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -881,13 +814,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId19"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId19"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -906,13 +839,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId20"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId20"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -931,13 +864,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId21"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId21"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -956,13 +889,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId22"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId22"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -981,13 +914,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId23"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId23"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1006,13 +939,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId24"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId24"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1031,13 +964,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId25"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId25"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1056,13 +989,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId26"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId26"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1081,13 +1014,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId27"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId27"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1106,13 +1039,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId28"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId28"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1131,13 +1064,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId29"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId29"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1156,13 +1089,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId30"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId30"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1181,13 +1114,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId31"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId31"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1206,13 +1139,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId32"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId32"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1231,13 +1164,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId33"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId33"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1256,13 +1189,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId34"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId34"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1281,13 +1214,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId35"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId35"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1306,13 +1239,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId36"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId36"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1331,13 +1264,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId37"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId37"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1356,13 +1289,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId38"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId38"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1381,13 +1314,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId39"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId39"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1406,13 +1339,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId40"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId40"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1431,13 +1364,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId41"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId41"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1456,13 +1389,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId42"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId42"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1481,13 +1414,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId43"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId43"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1506,13 +1439,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId44"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId44"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -1782,7 +1715,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -1796,7 +1729,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="95" t="n"/>
+      <c r="A1" s="95" t="inlineStr">
+        <is>
+          <t>DATE</t>
+        </is>
+      </c>
       <c r="B1" s="96" t="inlineStr">
         <is>
           <t>TMP</t>
@@ -1861,23 +1798,23 @@
     <row r="2">
       <c r="A2" s="95" t="inlineStr">
         <is>
-          <t>2021-12-14 15:00 mar</t>
-        </is>
-      </c>
-      <c r="B2" s="97" t="n">
-        <v>10</v>
-      </c>
-      <c r="C2" s="97" t="n">
-        <v>3</v>
-      </c>
-      <c r="D2" s="97" t="n">
-        <v>63</v>
-      </c>
-      <c r="E2" s="98" t="n">
-        <v>29</v>
+          <t xml:space="preserve">2021-12-29 03:00 Wed Wed </t>
+        </is>
+      </c>
+      <c r="B2" s="101" t="n">
+        <v>11</v>
+      </c>
+      <c r="C2" s="98" t="n">
+        <v>8</v>
+      </c>
+      <c r="D2" s="104" t="n">
+        <v>84</v>
+      </c>
+      <c r="E2" s="100" t="n">
+        <v>9</v>
       </c>
       <c r="F2" s="95" t="n">
-        <v>2</v>
+        <v>252</v>
       </c>
       <c r="G2" s="100" t="inlineStr">
         <is>
@@ -1899,42 +1836,42 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K2" s="100" t="inlineStr">
-        <is>
-          <t>2.4</t>
-        </is>
-      </c>
-      <c r="L2" s="95" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M2" s="100" t="inlineStr">
-        <is>
-          <t>0.4</t>
+      <c r="K2" s="108" t="inlineStr">
+        <is>
+          <t>6.1</t>
+        </is>
+      </c>
+      <c r="L2" s="101" t="inlineStr">
+        <is>
+          <t>28.9</t>
+        </is>
+      </c>
+      <c r="M2" s="103" t="inlineStr">
+        <is>
+          <t>70.7</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="95" t="inlineStr">
         <is>
-          <t>2021-12-14 18:00 mar</t>
+          <t xml:space="preserve">2021-12-29 06:00 Wed Wed </t>
         </is>
       </c>
       <c r="B3" s="97" t="n">
-        <v>9</v>
-      </c>
-      <c r="C3" s="97" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" s="97" t="n">
-        <v>64</v>
-      </c>
-      <c r="E3" s="98" t="n">
-        <v>23</v>
+        <v>10</v>
+      </c>
+      <c r="C3" s="98" t="n">
+        <v>8</v>
+      </c>
+      <c r="D3" s="104" t="n">
+        <v>87</v>
+      </c>
+      <c r="E3" s="99" t="n">
+        <v>12</v>
       </c>
       <c r="F3" s="95" t="n">
-        <v>3</v>
+        <v>233</v>
       </c>
       <c r="G3" s="100" t="inlineStr">
         <is>
@@ -1956,42 +1893,42 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K3" s="100" t="inlineStr">
-        <is>
-          <t>1.9</t>
-        </is>
-      </c>
-      <c r="L3" s="95" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M3" s="100" t="inlineStr">
-        <is>
-          <t>0.2</t>
+      <c r="K3" s="108" t="inlineStr">
+        <is>
+          <t>5.5</t>
+        </is>
+      </c>
+      <c r="L3" s="106" t="inlineStr">
+        <is>
+          <t>16.8</t>
+        </is>
+      </c>
+      <c r="M3" s="95" t="inlineStr">
+        <is>
+          <t>83.2</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="95" t="inlineStr">
         <is>
-          <t>2021-12-14 21:00 mar</t>
-        </is>
-      </c>
-      <c r="B4" s="97" t="n">
-        <v>8</v>
-      </c>
-      <c r="C4" s="97" t="n">
-        <v>3</v>
-      </c>
-      <c r="D4" s="97" t="n">
-        <v>67</v>
-      </c>
-      <c r="E4" s="98" t="n">
-        <v>22</v>
+          <t xml:space="preserve">2021-12-29 09:00 Wed Wed </t>
+        </is>
+      </c>
+      <c r="B4" s="98" t="n">
+        <v>14</v>
+      </c>
+      <c r="C4" s="98" t="n">
+        <v>9</v>
+      </c>
+      <c r="D4" s="104" t="n">
+        <v>72</v>
+      </c>
+      <c r="E4" s="99" t="n">
+        <v>11</v>
       </c>
       <c r="F4" s="95" t="n">
-        <v>4</v>
+        <v>273</v>
       </c>
       <c r="G4" s="100" t="inlineStr">
         <is>
@@ -2013,42 +1950,42 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K4" s="95" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L4" s="95" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M4" s="95" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K4" s="100" t="inlineStr">
+        <is>
+          <t>1.4</t>
+        </is>
+      </c>
+      <c r="L4" s="102" t="inlineStr">
+        <is>
+          <t>36.1</t>
+        </is>
+      </c>
+      <c r="M4" s="100" t="inlineStr">
+        <is>
+          <t>0.8</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="95" t="inlineStr">
         <is>
-          <t>2021-12-15 00:00 mer</t>
-        </is>
-      </c>
-      <c r="B5" s="97" t="n">
-        <v>9</v>
-      </c>
-      <c r="C5" s="97" t="n">
-        <v>2</v>
-      </c>
-      <c r="D5" s="97" t="n">
-        <v>65</v>
-      </c>
-      <c r="E5" s="98" t="n">
-        <v>27</v>
+          <t xml:space="preserve">2021-12-29 12:00 Wed Wed </t>
+        </is>
+      </c>
+      <c r="B5" s="98" t="n">
+        <v>16</v>
+      </c>
+      <c r="C5" s="98" t="n">
+        <v>8</v>
+      </c>
+      <c r="D5" s="98" t="n">
+        <v>59</v>
+      </c>
+      <c r="E5" s="99" t="n">
+        <v>13</v>
       </c>
       <c r="F5" s="95" t="n">
-        <v>8</v>
+        <v>310</v>
       </c>
       <c r="G5" s="100" t="inlineStr">
         <is>
@@ -2070,42 +2007,42 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K5" s="95" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L5" s="95" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M5" s="95" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K5" s="100" t="inlineStr">
+        <is>
+          <t>3.2</t>
+        </is>
+      </c>
+      <c r="L5" s="106" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="M5" s="100" t="inlineStr">
+        <is>
+          <t>0.4</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="95" t="inlineStr">
         <is>
-          <t>2021-12-15 03:00 mer</t>
-        </is>
-      </c>
-      <c r="B6" s="97" t="n">
-        <v>8</v>
-      </c>
-      <c r="C6" s="97" t="n">
-        <v>2</v>
-      </c>
-      <c r="D6" s="97" t="n">
-        <v>65</v>
-      </c>
-      <c r="E6" s="98" t="n">
-        <v>25</v>
+          <t xml:space="preserve">2021-12-29 15:00 Wed Wed </t>
+        </is>
+      </c>
+      <c r="B6" s="101" t="n">
+        <v>13</v>
+      </c>
+      <c r="C6" s="98" t="n">
+        <v>9</v>
+      </c>
+      <c r="D6" s="104" t="n">
+        <v>76</v>
+      </c>
+      <c r="E6" s="99" t="n">
+        <v>13</v>
       </c>
       <c r="F6" s="95" t="n">
-        <v>357</v>
+        <v>334</v>
       </c>
       <c r="G6" s="100" t="inlineStr">
         <is>
@@ -2127,9 +2064,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K6" s="95" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K6" s="100" t="inlineStr">
+        <is>
+          <t>3.4</t>
         </is>
       </c>
       <c r="L6" s="95" t="inlineStr">
@@ -2137,32 +2074,32 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M6" s="95" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M6" s="100" t="inlineStr">
+        <is>
+          <t>0.5</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="95" t="inlineStr">
         <is>
-          <t>2021-12-15 06:00 mer</t>
-        </is>
-      </c>
-      <c r="B7" s="97" t="n">
-        <v>7</v>
-      </c>
-      <c r="C7" s="97" t="n">
-        <v>3</v>
+          <t xml:space="preserve">2021-12-29 18:00 Wed Wed </t>
+        </is>
+      </c>
+      <c r="B7" s="101" t="n">
+        <v>11</v>
+      </c>
+      <c r="C7" s="98" t="n">
+        <v>9</v>
       </c>
       <c r="D7" s="104" t="n">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="E7" s="99" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F7" s="95" t="n">
-        <v>345</v>
+        <v>333</v>
       </c>
       <c r="G7" s="100" t="inlineStr">
         <is>
@@ -2184,9 +2121,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K7" s="95" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K7" s="100" t="inlineStr">
+        <is>
+          <t>4.3</t>
         </is>
       </c>
       <c r="L7" s="95" t="inlineStr">
@@ -2194,41 +2131,41 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M7" s="95" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M7" s="108" t="inlineStr">
+        <is>
+          <t>6.1</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="95" t="inlineStr">
         <is>
-          <t>2021-12-15 09:00 mer</t>
+          <t xml:space="preserve">2021-12-29 21:00 Wed Wed </t>
         </is>
       </c>
       <c r="B8" s="101" t="n">
         <v>11</v>
       </c>
-      <c r="C8" s="97" t="n">
-        <v>4</v>
-      </c>
-      <c r="D8" s="97" t="n">
-        <v>61</v>
+      <c r="C8" s="98" t="n">
+        <v>10</v>
+      </c>
+      <c r="D8" s="104" t="n">
+        <v>90</v>
       </c>
       <c r="E8" s="99" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F8" s="95" t="n">
-        <v>2</v>
-      </c>
-      <c r="G8" s="100" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="H8" s="100" t="inlineStr">
-        <is>
-          <t>0</t>
+        <v>340</v>
+      </c>
+      <c r="G8" s="99" t="inlineStr">
+        <is>
+          <t>7.2e-06</t>
+        </is>
+      </c>
+      <c r="H8" s="98" t="inlineStr">
+        <is>
+          <t>1</t>
         </is>
       </c>
       <c r="I8" s="100" t="inlineStr">
@@ -2241,9 +2178,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K8" s="95" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K8" s="100" t="inlineStr">
+        <is>
+          <t>1.7</t>
         </is>
       </c>
       <c r="L8" s="95" t="inlineStr">
@@ -2251,36 +2188,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M8" s="95" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M8" s="108" t="inlineStr">
+        <is>
+          <t>10</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="95" t="inlineStr">
         <is>
-          <t>2021-12-15 12:00 mer</t>
+          <t xml:space="preserve">2021-12-30 00:00 Thu Thu </t>
         </is>
       </c>
       <c r="B9" s="101" t="n">
-        <v>12</v>
-      </c>
-      <c r="C9" s="97" t="n">
-        <v>4</v>
-      </c>
-      <c r="D9" s="98" t="n">
-        <v>57</v>
+        <v>11</v>
+      </c>
+      <c r="C9" s="98" t="n">
+        <v>9</v>
+      </c>
+      <c r="D9" s="104" t="n">
+        <v>87</v>
       </c>
       <c r="E9" s="98" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F9" s="95" t="n">
-        <v>343</v>
-      </c>
-      <c r="G9" s="100" t="inlineStr">
-        <is>
-          <t>0</t>
+        <v>347</v>
+      </c>
+      <c r="G9" s="99" t="inlineStr">
+        <is>
+          <t>1.6e-06</t>
         </is>
       </c>
       <c r="H9" s="100" t="inlineStr">
@@ -2298,9 +2235,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K9" s="95" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K9" s="100" t="inlineStr">
+        <is>
+          <t>1.2</t>
         </is>
       </c>
       <c r="L9" s="95" t="inlineStr">
@@ -2308,36 +2245,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M9" s="100" t="inlineStr">
-        <is>
-          <t>0.8</t>
+      <c r="M9" s="108" t="inlineStr">
+        <is>
+          <t>5</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="95" t="inlineStr">
         <is>
-          <t>2021-12-15 15:00 mer</t>
-        </is>
-      </c>
-      <c r="B10" s="97" t="n">
-        <v>10</v>
-      </c>
-      <c r="C10" s="97" t="n">
-        <v>4</v>
-      </c>
-      <c r="D10" s="97" t="n">
-        <v>68</v>
-      </c>
-      <c r="E10" s="99" t="n">
-        <v>15</v>
+          <t xml:space="preserve">2021-12-30 03:00 Thu Thu </t>
+        </is>
+      </c>
+      <c r="B10" s="101" t="n">
+        <v>11</v>
+      </c>
+      <c r="C10" s="98" t="n">
+        <v>9</v>
+      </c>
+      <c r="D10" s="104" t="n">
+        <v>84</v>
+      </c>
+      <c r="E10" s="98" t="n">
+        <v>27</v>
       </c>
       <c r="F10" s="95" t="n">
-        <v>346</v>
-      </c>
-      <c r="G10" s="100" t="inlineStr">
-        <is>
-          <t>0</t>
+        <v>345</v>
+      </c>
+      <c r="G10" s="99" t="inlineStr">
+        <is>
+          <t>2e-06</t>
         </is>
       </c>
       <c r="H10" s="100" t="inlineStr">
@@ -2367,34 +2304,34 @@
       </c>
       <c r="M10" s="100" t="inlineStr">
         <is>
-          <t>3.3</t>
+          <t>0.4</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="95" t="inlineStr">
         <is>
-          <t>2021-12-15 18:00 mer</t>
-        </is>
-      </c>
-      <c r="B11" s="97" t="n">
-        <v>8</v>
-      </c>
-      <c r="C11" s="97" t="n">
-        <v>4</v>
+          <t xml:space="preserve">2021-12-30 06:00 Thu Thu </t>
+        </is>
+      </c>
+      <c r="B11" s="101" t="n">
+        <v>11</v>
+      </c>
+      <c r="C11" s="98" t="n">
+        <v>9</v>
       </c>
       <c r="D11" s="104" t="n">
-        <v>76</v>
-      </c>
-      <c r="E11" s="99" t="n">
-        <v>12</v>
+        <v>86</v>
+      </c>
+      <c r="E11" s="98" t="n">
+        <v>33</v>
       </c>
       <c r="F11" s="95" t="n">
-        <v>345</v>
-      </c>
-      <c r="G11" s="100" t="inlineStr">
-        <is>
-          <t>0</t>
+        <v>344</v>
+      </c>
+      <c r="G11" s="99" t="inlineStr">
+        <is>
+          <t>1.2e-06</t>
         </is>
       </c>
       <c r="H11" s="100" t="inlineStr">
@@ -2412,42 +2349,42 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K11" s="95" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L11" s="100" t="inlineStr">
-        <is>
-          <t>0.6</t>
-        </is>
-      </c>
-      <c r="M11" s="108" t="inlineStr">
-        <is>
-          <t>10</t>
+      <c r="K11" s="100" t="inlineStr">
+        <is>
+          <t>3.6</t>
+        </is>
+      </c>
+      <c r="L11" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M11" s="106" t="inlineStr">
+        <is>
+          <t>17.7</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="95" t="inlineStr">
         <is>
-          <t>2021-12-15 21:00 mer</t>
-        </is>
-      </c>
-      <c r="B12" s="97" t="n">
-        <v>8</v>
-      </c>
-      <c r="C12" s="97" t="n">
-        <v>4</v>
+          <t xml:space="preserve">2021-12-30 09:00 Thu Thu </t>
+        </is>
+      </c>
+      <c r="B12" s="101" t="n">
+        <v>13</v>
+      </c>
+      <c r="C12" s="98" t="n">
+        <v>9</v>
       </c>
       <c r="D12" s="104" t="n">
-        <v>76</v>
-      </c>
-      <c r="E12" s="99" t="n">
-        <v>10</v>
+        <v>75</v>
+      </c>
+      <c r="E12" s="98" t="n">
+        <v>34</v>
       </c>
       <c r="F12" s="95" t="n">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="G12" s="100" t="inlineStr">
         <is>
@@ -2469,9 +2406,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K12" s="95" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K12" s="108" t="inlineStr">
+        <is>
+          <t>9.6</t>
         </is>
       </c>
       <c r="L12" s="95" t="inlineStr">
@@ -2479,32 +2416,32 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M12" s="95" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M12" s="105" t="inlineStr">
+        <is>
+          <t>99.8</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="95" t="inlineStr">
         <is>
-          <t>2021-12-16 00:00 gio</t>
-        </is>
-      </c>
-      <c r="B13" s="97" t="n">
-        <v>8</v>
-      </c>
-      <c r="C13" s="97" t="n">
-        <v>3</v>
+          <t xml:space="preserve">2021-12-30 12:00 Thu Thu </t>
+        </is>
+      </c>
+      <c r="B13" s="98" t="n">
+        <v>14</v>
+      </c>
+      <c r="C13" s="98" t="n">
+        <v>7</v>
       </c>
       <c r="D13" s="97" t="n">
-        <v>70</v>
-      </c>
-      <c r="E13" s="99" t="n">
-        <v>14</v>
+        <v>62</v>
+      </c>
+      <c r="E13" s="98" t="n">
+        <v>35</v>
       </c>
       <c r="F13" s="95" t="n">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="G13" s="100" t="inlineStr">
         <is>
@@ -2526,9 +2463,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K13" s="95" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K13" s="100" t="inlineStr">
+        <is>
+          <t>4.8</t>
         </is>
       </c>
       <c r="L13" s="95" t="inlineStr">
@@ -2536,32 +2473,32 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M13" s="100" t="inlineStr">
-        <is>
-          <t>0.8</t>
+      <c r="M13" s="102" t="inlineStr">
+        <is>
+          <t>52.3</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="95" t="inlineStr">
         <is>
-          <t>2021-12-16 03:00 gio</t>
-        </is>
-      </c>
-      <c r="B14" s="97" t="n">
-        <v>7</v>
-      </c>
-      <c r="C14" s="97" t="n">
-        <v>3</v>
-      </c>
-      <c r="D14" s="104" t="n">
-        <v>72</v>
-      </c>
-      <c r="E14" s="99" t="n">
-        <v>13</v>
+          <t xml:space="preserve">2021-12-30 15:00 Thu Thu </t>
+        </is>
+      </c>
+      <c r="B14" s="101" t="n">
+        <v>12</v>
+      </c>
+      <c r="C14" s="98" t="n">
+        <v>6</v>
+      </c>
+      <c r="D14" s="97" t="n">
+        <v>67</v>
+      </c>
+      <c r="E14" s="98" t="n">
+        <v>27</v>
       </c>
       <c r="F14" s="95" t="n">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G14" s="100" t="inlineStr">
         <is>
@@ -2593,32 +2530,32 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M14" s="100" t="inlineStr">
-        <is>
-          <t>3.7</t>
+      <c r="M14" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="95" t="inlineStr">
         <is>
-          <t>2021-12-16 06:00 gio</t>
-        </is>
-      </c>
-      <c r="B15" s="97" t="n">
-        <v>7</v>
+          <t xml:space="preserve">2021-12-30 18:00 Thu Thu </t>
+        </is>
+      </c>
+      <c r="B15" s="101" t="n">
+        <v>11</v>
       </c>
       <c r="C15" s="97" t="n">
-        <v>2</v>
-      </c>
-      <c r="D15" s="104" t="n">
-        <v>71</v>
-      </c>
-      <c r="E15" s="99" t="n">
-        <v>13</v>
+        <v>5</v>
+      </c>
+      <c r="D15" s="97" t="n">
+        <v>65</v>
+      </c>
+      <c r="E15" s="98" t="n">
+        <v>30</v>
       </c>
       <c r="F15" s="95" t="n">
-        <v>347</v>
+        <v>6</v>
       </c>
       <c r="G15" s="100" t="inlineStr">
         <is>
@@ -2650,32 +2587,32 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M15" s="100" t="inlineStr">
-        <is>
-          <t>1.9</t>
+      <c r="M15" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="95" t="inlineStr">
         <is>
-          <t>2021-12-16 09:00 gio</t>
+          <t xml:space="preserve">2021-12-30 21:00 Thu Thu </t>
         </is>
       </c>
       <c r="B16" s="101" t="n">
         <v>11</v>
       </c>
       <c r="C16" s="97" t="n">
+        <v>5</v>
+      </c>
+      <c r="D16" s="97" t="n">
+        <v>65</v>
+      </c>
+      <c r="E16" s="98" t="n">
+        <v>30</v>
+      </c>
+      <c r="F16" s="95" t="n">
         <v>3</v>
-      </c>
-      <c r="D16" s="98" t="n">
-        <v>58</v>
-      </c>
-      <c r="E16" s="98" t="n">
-        <v>21</v>
-      </c>
-      <c r="F16" s="95" t="n">
-        <v>7</v>
       </c>
       <c r="G16" s="100" t="inlineStr">
         <is>
@@ -2716,23 +2653,23 @@
     <row r="17">
       <c r="A17" s="95" t="inlineStr">
         <is>
-          <t>2021-12-16 12:00 gio</t>
+          <t xml:space="preserve">2021-12-31 00:00 Fri Fri </t>
         </is>
       </c>
       <c r="B17" s="101" t="n">
         <v>11</v>
       </c>
       <c r="C17" s="97" t="n">
-        <v>2</v>
-      </c>
-      <c r="D17" s="98" t="n">
-        <v>55</v>
-      </c>
-      <c r="E17" s="99" t="n">
-        <v>20</v>
+        <v>4</v>
+      </c>
+      <c r="D17" s="97" t="n">
+        <v>65</v>
+      </c>
+      <c r="E17" s="98" t="n">
+        <v>30</v>
       </c>
       <c r="F17" s="95" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G17" s="100" t="inlineStr">
         <is>
@@ -2773,23 +2710,23 @@
     <row r="18">
       <c r="A18" s="95" t="inlineStr">
         <is>
-          <t>2021-12-16 15:00 gio</t>
+          <t xml:space="preserve">2021-12-31 03:00 Fri Fri </t>
         </is>
       </c>
       <c r="B18" s="97" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C18" s="97" t="n">
         <v>4</v>
       </c>
       <c r="D18" s="97" t="n">
-        <v>69</v>
-      </c>
-      <c r="E18" s="99" t="n">
-        <v>14</v>
+        <v>67</v>
+      </c>
+      <c r="E18" s="98" t="n">
+        <v>25</v>
       </c>
       <c r="F18" s="95" t="n">
-        <v>353</v>
+        <v>2</v>
       </c>
       <c r="G18" s="100" t="inlineStr">
         <is>
@@ -2811,9 +2748,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K18" s="100" t="inlineStr">
-        <is>
-          <t>0.1</t>
+      <c r="K18" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L18" s="95" t="inlineStr">
@@ -2821,32 +2758,32 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M18" s="95" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M18" s="100" t="inlineStr">
+        <is>
+          <t>1.7</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="95" t="inlineStr">
         <is>
-          <t>2021-12-16 18:00 gio</t>
+          <t xml:space="preserve">2021-12-31 06:00 Fri Fri </t>
         </is>
       </c>
       <c r="B19" s="97" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C19" s="97" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D19" s="104" t="n">
-        <v>78</v>
-      </c>
-      <c r="E19" s="99" t="n">
-        <v>11</v>
+        <v>71</v>
+      </c>
+      <c r="E19" s="98" t="n">
+        <v>21</v>
       </c>
       <c r="F19" s="95" t="n">
-        <v>355</v>
+        <v>2</v>
       </c>
       <c r="G19" s="100" t="inlineStr">
         <is>
@@ -2868,9 +2805,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K19" s="100" t="inlineStr">
-        <is>
-          <t>1.3</t>
+      <c r="K19" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L19" s="95" t="inlineStr">
@@ -2887,23 +2824,23 @@
     <row r="20">
       <c r="A20" s="95" t="inlineStr">
         <is>
-          <t>2021-12-16 21:00 gio</t>
-        </is>
-      </c>
-      <c r="B20" s="97" t="n">
-        <v>7</v>
-      </c>
-      <c r="C20" s="97" t="n">
-        <v>4</v>
-      </c>
-      <c r="D20" s="104" t="n">
-        <v>79</v>
-      </c>
-      <c r="E20" s="99" t="n">
-        <v>11</v>
+          <t xml:space="preserve">2021-12-31 09:00 Fri Fri </t>
+        </is>
+      </c>
+      <c r="B20" s="101" t="n">
+        <v>13</v>
+      </c>
+      <c r="C20" s="98" t="n">
+        <v>6</v>
+      </c>
+      <c r="D20" s="97" t="n">
+        <v>63</v>
+      </c>
+      <c r="E20" s="98" t="n">
+        <v>21</v>
       </c>
       <c r="F20" s="95" t="n">
-        <v>312</v>
+        <v>2</v>
       </c>
       <c r="G20" s="100" t="inlineStr">
         <is>
@@ -2925,9 +2862,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K20" s="106" t="inlineStr">
-        <is>
-          <t>11.5</t>
+      <c r="K20" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L20" s="95" t="inlineStr">
@@ -2944,27 +2881,27 @@
     <row r="21">
       <c r="A21" s="95" t="inlineStr">
         <is>
-          <t>2021-12-17 00:00 ven</t>
-        </is>
-      </c>
-      <c r="B21" s="97" t="n">
-        <v>9</v>
-      </c>
-      <c r="C21" s="97" t="n">
-        <v>4</v>
-      </c>
-      <c r="D21" s="104" t="n">
-        <v>75</v>
-      </c>
-      <c r="E21" s="99" t="n">
-        <v>11</v>
+          <t xml:space="preserve">2021-12-31 12:00 Fri Fri </t>
+        </is>
+      </c>
+      <c r="B21" s="98" t="n">
+        <v>14</v>
+      </c>
+      <c r="C21" s="98" t="n">
+        <v>6</v>
+      </c>
+      <c r="D21" s="98" t="n">
+        <v>59</v>
+      </c>
+      <c r="E21" s="98" t="n">
+        <v>23</v>
       </c>
       <c r="F21" s="95" t="n">
-        <v>318</v>
-      </c>
-      <c r="G21" s="99" t="inlineStr">
-        <is>
-          <t>2.8e-06</t>
+        <v>354</v>
+      </c>
+      <c r="G21" s="100" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="H21" s="100" t="inlineStr">
@@ -2982,42 +2919,42 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K21" s="102" t="inlineStr">
-        <is>
-          <t>47.9</t>
-        </is>
-      </c>
-      <c r="L21" s="106" t="inlineStr">
-        <is>
-          <t>10.8</t>
-        </is>
-      </c>
-      <c r="M21" s="106" t="inlineStr">
-        <is>
-          <t>16.3</t>
+      <c r="K21" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L21" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M21" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="95" t="inlineStr">
         <is>
-          <t>2021-12-17 03:00 ven</t>
-        </is>
-      </c>
-      <c r="B22" s="97" t="n">
-        <v>8</v>
-      </c>
-      <c r="C22" s="97" t="n">
-        <v>3</v>
+          <t xml:space="preserve">2021-12-31 15:00 Fri Fri </t>
+        </is>
+      </c>
+      <c r="B22" s="101" t="n">
+        <v>12</v>
+      </c>
+      <c r="C22" s="98" t="n">
+        <v>7</v>
       </c>
       <c r="D22" s="104" t="n">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E22" s="99" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F22" s="95" t="n">
-        <v>7</v>
+        <v>356</v>
       </c>
       <c r="G22" s="100" t="inlineStr">
         <is>
@@ -3039,42 +2976,42 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K22" s="105" t="inlineStr">
-        <is>
-          <t>80.2</t>
-        </is>
-      </c>
-      <c r="L22" s="102" t="inlineStr">
-        <is>
-          <t>49.5</t>
-        </is>
-      </c>
-      <c r="M22" s="102" t="inlineStr">
-        <is>
-          <t>45.4</t>
+      <c r="K22" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L22" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M22" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="95" t="inlineStr">
         <is>
-          <t>2021-12-17 06:00 ven</t>
+          <t xml:space="preserve">2021-12-31 18:00 Fri Fri </t>
         </is>
       </c>
       <c r="B23" s="97" t="n">
-        <v>7</v>
-      </c>
-      <c r="C23" s="97" t="n">
-        <v>3</v>
+        <v>10</v>
+      </c>
+      <c r="C23" s="98" t="n">
+        <v>8</v>
       </c>
       <c r="D23" s="104" t="n">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="E23" s="99" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F23" s="95" t="n">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="G23" s="100" t="inlineStr">
         <is>
@@ -3096,42 +3033,42 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K23" s="102" t="inlineStr">
-        <is>
-          <t>46.1</t>
-        </is>
-      </c>
-      <c r="L23" s="101" t="inlineStr">
-        <is>
-          <t>28</t>
-        </is>
-      </c>
-      <c r="M23" s="101" t="inlineStr">
-        <is>
-          <t>24.1</t>
+      <c r="K23" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L23" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M23" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="95" t="inlineStr">
         <is>
-          <t>2021-12-17 09:00 ven</t>
-        </is>
-      </c>
-      <c r="B24" s="101" t="n">
-        <v>11</v>
-      </c>
-      <c r="C24" s="97" t="n">
-        <v>3</v>
-      </c>
-      <c r="D24" s="98" t="n">
-        <v>58</v>
-      </c>
-      <c r="E24" s="98" t="n">
-        <v>22</v>
+          <t xml:space="preserve">2021-12-31 21:00 Fri Fri </t>
+        </is>
+      </c>
+      <c r="B24" s="97" t="n">
+        <v>10</v>
+      </c>
+      <c r="C24" s="98" t="n">
+        <v>8</v>
+      </c>
+      <c r="D24" s="104" t="n">
+        <v>88</v>
+      </c>
+      <c r="E24" s="99" t="n">
+        <v>12</v>
       </c>
       <c r="F24" s="95" t="n">
-        <v>4</v>
+        <v>329</v>
       </c>
       <c r="G24" s="100" t="inlineStr">
         <is>
@@ -3153,42 +3090,42 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K24" s="108" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="L24" s="100" t="inlineStr">
-        <is>
-          <t>1.7</t>
-        </is>
-      </c>
-      <c r="M24" s="101" t="inlineStr">
-        <is>
-          <t>27.9</t>
+      <c r="K24" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L24" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M24" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="95" t="inlineStr">
         <is>
-          <t>2021-12-17 12:00 ven</t>
-        </is>
-      </c>
-      <c r="B25" s="101" t="n">
-        <v>12</v>
-      </c>
-      <c r="C25" s="97" t="n">
-        <v>4</v>
-      </c>
-      <c r="D25" s="98" t="n">
-        <v>56</v>
-      </c>
-      <c r="E25" s="98" t="n">
-        <v>25</v>
+          <t xml:space="preserve">2022-01-01 00:00 Sat Sat </t>
+        </is>
+      </c>
+      <c r="B25" s="97" t="n">
+        <v>10</v>
+      </c>
+      <c r="C25" s="98" t="n">
+        <v>9</v>
+      </c>
+      <c r="D25" s="104" t="n">
+        <v>94</v>
+      </c>
+      <c r="E25" s="99" t="n">
+        <v>11</v>
       </c>
       <c r="F25" s="95" t="n">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="G25" s="100" t="inlineStr">
         <is>
@@ -3210,42 +3147,42 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K25" s="108" t="inlineStr">
-        <is>
-          <t>7.6</t>
-        </is>
-      </c>
-      <c r="L25" s="100" t="inlineStr">
-        <is>
-          <t>0.8</t>
-        </is>
-      </c>
-      <c r="M25" s="102" t="inlineStr">
-        <is>
-          <t>33.2</t>
+      <c r="K25" s="100" t="inlineStr">
+        <is>
+          <t>0.1</t>
+        </is>
+      </c>
+      <c r="L25" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M25" s="100" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="95" t="inlineStr">
         <is>
-          <t>2021-12-17 15:00 ven</t>
+          <t xml:space="preserve">2022-01-01 03:00 Sat Sat </t>
         </is>
       </c>
       <c r="B26" s="97" t="n">
         <v>10</v>
       </c>
-      <c r="C26" s="97" t="n">
-        <v>5</v>
-      </c>
-      <c r="D26" s="97" t="n">
-        <v>67</v>
+      <c r="C26" s="98" t="n">
+        <v>10</v>
+      </c>
+      <c r="D26" s="104" t="n">
+        <v>96</v>
       </c>
       <c r="E26" s="99" t="n">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F26" s="95" t="n">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="G26" s="100" t="inlineStr">
         <is>
@@ -3267,9 +3204,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K26" s="95" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K26" s="100" t="inlineStr">
+        <is>
+          <t>2.6</t>
         </is>
       </c>
       <c r="L26" s="95" t="inlineStr">
@@ -3277,36 +3214,36 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M26" s="95" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M26" s="102" t="inlineStr">
+        <is>
+          <t>55.8</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="95" t="inlineStr">
         <is>
-          <t>2021-12-17 18:00 ven</t>
+          <t xml:space="preserve">2022-01-01 06:00 Sat Sat </t>
         </is>
       </c>
       <c r="B27" s="97" t="n">
         <v>10</v>
       </c>
       <c r="C27" s="98" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D27" s="104" t="n">
-        <v>75</v>
-      </c>
-      <c r="E27" s="98" t="n">
-        <v>24</v>
+        <v>96</v>
+      </c>
+      <c r="E27" s="99" t="n">
+        <v>12</v>
       </c>
       <c r="F27" s="95" t="n">
-        <v>328</v>
-      </c>
-      <c r="G27" s="99" t="inlineStr">
-        <is>
-          <t>4.8e-06</t>
+        <v>337</v>
+      </c>
+      <c r="G27" s="100" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="H27" s="100" t="inlineStr">
@@ -3326,40 +3263,40 @@
       </c>
       <c r="K27" s="100" t="inlineStr">
         <is>
-          <t>3.5</t>
-        </is>
-      </c>
-      <c r="L27" s="95" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M27" s="95" t="inlineStr">
-        <is>
-          <t>0</t>
+          <t>2.6</t>
+        </is>
+      </c>
+      <c r="L27" s="100" t="inlineStr">
+        <is>
+          <t>0.8</t>
+        </is>
+      </c>
+      <c r="M27" s="102" t="inlineStr">
+        <is>
+          <t>31.2</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="95" t="inlineStr">
         <is>
-          <t>2021-12-17 21:00 ven</t>
-        </is>
-      </c>
-      <c r="B28" s="97" t="n">
-        <v>10</v>
-      </c>
-      <c r="C28" s="97" t="n">
-        <v>4</v>
-      </c>
-      <c r="D28" s="97" t="n">
-        <v>62</v>
-      </c>
-      <c r="E28" s="98" t="n">
-        <v>29</v>
+          <t xml:space="preserve">2022-01-01 09:00 Sat Sat </t>
+        </is>
+      </c>
+      <c r="B28" s="98" t="n">
+        <v>14</v>
+      </c>
+      <c r="C28" s="107" t="n">
+        <v>11</v>
+      </c>
+      <c r="D28" s="104" t="n">
+        <v>81</v>
+      </c>
+      <c r="E28" s="99" t="n">
+        <v>20</v>
       </c>
       <c r="F28" s="95" t="n">
-        <v>335</v>
+        <v>347</v>
       </c>
       <c r="G28" s="100" t="inlineStr">
         <is>
@@ -3381,42 +3318,42 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K28" s="102" t="inlineStr">
-        <is>
-          <t>40.6</t>
-        </is>
-      </c>
-      <c r="L28" s="100" t="inlineStr">
-        <is>
-          <t>2.9</t>
-        </is>
-      </c>
-      <c r="M28" s="102" t="inlineStr">
-        <is>
-          <t>38.8</t>
+      <c r="K28" s="106" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="L28" s="106" t="inlineStr">
+        <is>
+          <t>19.1</t>
+        </is>
+      </c>
+      <c r="M28" s="100" t="inlineStr">
+        <is>
+          <t>4.1</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="95" t="inlineStr">
         <is>
-          <t>2021-12-18 00:00 sab</t>
-        </is>
-      </c>
-      <c r="B29" s="97" t="n">
+          <t xml:space="preserve">2022-01-01 12:00 Sat Sat </t>
+        </is>
+      </c>
+      <c r="B29" s="98" t="n">
+        <v>15</v>
+      </c>
+      <c r="C29" s="98" t="n">
         <v>10</v>
       </c>
-      <c r="C29" s="97" t="n">
-        <v>1</v>
-      </c>
-      <c r="D29" s="98" t="n">
-        <v>51</v>
+      <c r="D29" s="104" t="n">
+        <v>71</v>
       </c>
       <c r="E29" s="98" t="n">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="F29" s="95" t="n">
-        <v>333</v>
+        <v>346</v>
       </c>
       <c r="G29" s="100" t="inlineStr">
         <is>
@@ -3438,42 +3375,42 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K29" s="106" t="inlineStr">
-        <is>
-          <t>20.3</t>
-        </is>
-      </c>
-      <c r="L29" s="100" t="inlineStr">
-        <is>
-          <t>2.3</t>
-        </is>
-      </c>
-      <c r="M29" s="101" t="inlineStr">
-        <is>
-          <t>23.4</t>
+      <c r="K29" s="108" t="inlineStr">
+        <is>
+          <t>6.6</t>
+        </is>
+      </c>
+      <c r="L29" s="108" t="inlineStr">
+        <is>
+          <t>9.5</t>
+        </is>
+      </c>
+      <c r="M29" s="100" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="95" t="inlineStr">
         <is>
-          <t>2021-12-18 03:00 sab</t>
-        </is>
-      </c>
-      <c r="B30" s="97" t="n">
-        <v>9</v>
-      </c>
-      <c r="C30" s="97" t="n">
-        <v>0</v>
-      </c>
-      <c r="D30" s="98" t="n">
-        <v>54</v>
+          <t xml:space="preserve">2022-01-01 15:00 Sat Sat </t>
+        </is>
+      </c>
+      <c r="B30" s="101" t="n">
+        <v>13</v>
+      </c>
+      <c r="C30" s="107" t="n">
+        <v>11</v>
+      </c>
+      <c r="D30" s="104" t="n">
+        <v>87</v>
       </c>
       <c r="E30" s="98" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F30" s="95" t="n">
-        <v>343</v>
+        <v>349</v>
       </c>
       <c r="G30" s="100" t="inlineStr">
         <is>
@@ -3495,42 +3432,42 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K30" s="100" t="inlineStr">
-        <is>
-          <t>3.1</t>
-        </is>
-      </c>
-      <c r="L30" s="102" t="inlineStr">
-        <is>
-          <t>58.6</t>
-        </is>
-      </c>
-      <c r="M30" s="105" t="inlineStr">
-        <is>
-          <t>96.9</t>
+      <c r="K30" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L30" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M30" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="95" t="inlineStr">
         <is>
-          <t>2021-12-18 06:00 sab</t>
-        </is>
-      </c>
-      <c r="B31" s="97" t="n">
-        <v>9</v>
-      </c>
-      <c r="C31" s="97" t="n">
-        <v>-3</v>
-      </c>
-      <c r="D31" s="98" t="n">
-        <v>41</v>
-      </c>
-      <c r="E31" s="98" t="n">
-        <v>35</v>
+          <t xml:space="preserve">2022-01-01 18:00 Sat Sat </t>
+        </is>
+      </c>
+      <c r="B31" s="101" t="n">
+        <v>11</v>
+      </c>
+      <c r="C31" s="98" t="n">
+        <v>10</v>
+      </c>
+      <c r="D31" s="104" t="n">
+        <v>91</v>
+      </c>
+      <c r="E31" s="99" t="n">
+        <v>15</v>
       </c>
       <c r="F31" s="95" t="n">
-        <v>353</v>
+        <v>340</v>
       </c>
       <c r="G31" s="100" t="inlineStr">
         <is>
@@ -3552,42 +3489,42 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K31" s="100" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="L31" s="103" t="inlineStr">
-        <is>
-          <t>62</t>
-        </is>
-      </c>
-      <c r="M31" s="95" t="inlineStr">
-        <is>
-          <t>81.8</t>
+      <c r="K31" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L31" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M31" s="100" t="inlineStr">
+        <is>
+          <t>0.9</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="95" t="inlineStr">
         <is>
-          <t>2021-12-18 09:00 sab</t>
-        </is>
-      </c>
-      <c r="B32" s="97" t="n">
-        <v>9</v>
-      </c>
-      <c r="C32" s="97" t="n">
-        <v>-2</v>
-      </c>
-      <c r="D32" s="98" t="n">
-        <v>43</v>
-      </c>
-      <c r="E32" s="98" t="n">
-        <v>39</v>
+          <t xml:space="preserve">2022-01-01 21:00 Sat Sat </t>
+        </is>
+      </c>
+      <c r="B32" s="101" t="n">
+        <v>11</v>
+      </c>
+      <c r="C32" s="98" t="n">
+        <v>10</v>
+      </c>
+      <c r="D32" s="104" t="n">
+        <v>92</v>
+      </c>
+      <c r="E32" s="99" t="n">
+        <v>15</v>
       </c>
       <c r="F32" s="95" t="n">
-        <v>7</v>
+        <v>335</v>
       </c>
       <c r="G32" s="100" t="inlineStr">
         <is>
@@ -3609,9 +3546,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K32" s="102" t="inlineStr">
-        <is>
-          <t>56.1</t>
+      <c r="K32" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L32" s="95" t="inlineStr">
@@ -3619,41 +3556,41 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M32" s="95" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M32" s="108" t="inlineStr">
+        <is>
+          <t>6.9</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="95" t="inlineStr">
         <is>
-          <t>2021-12-18 12:00 sab</t>
-        </is>
-      </c>
-      <c r="B33" s="97" t="n">
-        <v>9</v>
-      </c>
-      <c r="C33" s="97" t="n">
-        <v>-2</v>
-      </c>
-      <c r="D33" s="98" t="n">
-        <v>42</v>
-      </c>
-      <c r="E33" s="98" t="n">
-        <v>42</v>
+          <t xml:space="preserve">2022-01-02 00:00 Sun Sun </t>
+        </is>
+      </c>
+      <c r="B33" s="101" t="n">
+        <v>12</v>
+      </c>
+      <c r="C33" s="98" t="n">
+        <v>10</v>
+      </c>
+      <c r="D33" s="104" t="n">
+        <v>91</v>
+      </c>
+      <c r="E33" s="99" t="n">
+        <v>20</v>
       </c>
       <c r="F33" s="95" t="n">
-        <v>13</v>
-      </c>
-      <c r="G33" s="99" t="inlineStr">
-        <is>
-          <t>3.52e-05</t>
-        </is>
-      </c>
-      <c r="H33" s="98" t="inlineStr">
-        <is>
-          <t>1</t>
+        <v>346</v>
+      </c>
+      <c r="G33" s="100" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H33" s="100" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="I33" s="100" t="inlineStr">
@@ -3666,9 +3603,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K33" s="103" t="inlineStr">
-        <is>
-          <t>63</t>
+      <c r="K33" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L33" s="95" t="inlineStr">
@@ -3676,32 +3613,32 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M33" s="95" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M33" s="101" t="inlineStr">
+        <is>
+          <t>23</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="95" t="inlineStr">
         <is>
-          <t>2021-12-18 15:00 sab</t>
-        </is>
-      </c>
-      <c r="B34" s="97" t="n">
-        <v>8</v>
-      </c>
-      <c r="C34" s="97" t="n">
-        <v>-2</v>
-      </c>
-      <c r="D34" s="98" t="n">
-        <v>47</v>
-      </c>
-      <c r="E34" s="98" t="n">
-        <v>29</v>
+          <t xml:space="preserve">2022-01-02 03:00 Sun Sun </t>
+        </is>
+      </c>
+      <c r="B34" s="101" t="n">
+        <v>11</v>
+      </c>
+      <c r="C34" s="98" t="n">
+        <v>10</v>
+      </c>
+      <c r="D34" s="104" t="n">
+        <v>93</v>
+      </c>
+      <c r="E34" s="99" t="n">
+        <v>18</v>
       </c>
       <c r="F34" s="95" t="n">
-        <v>21</v>
+        <v>343</v>
       </c>
       <c r="G34" s="100" t="inlineStr">
         <is>
@@ -3723,9 +3660,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K34" s="108" t="inlineStr">
-        <is>
-          <t>6</t>
+      <c r="K34" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L34" s="100" t="inlineStr">
@@ -3733,32 +3670,32 @@
           <t>1.7</t>
         </is>
       </c>
-      <c r="M34" s="95" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M34" s="100" t="inlineStr">
+        <is>
+          <t>3.1</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="95" t="inlineStr">
         <is>
-          <t>2021-12-18 18:00 sab</t>
-        </is>
-      </c>
-      <c r="B35" s="97" t="n">
-        <v>7</v>
-      </c>
-      <c r="C35" s="97" t="n">
-        <v>-2</v>
-      </c>
-      <c r="D35" s="98" t="n">
-        <v>47</v>
-      </c>
-      <c r="E35" s="98" t="n">
-        <v>39</v>
+          <t xml:space="preserve">2022-01-02 06:00 Sun Sun </t>
+        </is>
+      </c>
+      <c r="B35" s="101" t="n">
+        <v>11</v>
+      </c>
+      <c r="C35" s="98" t="n">
+        <v>10</v>
+      </c>
+      <c r="D35" s="104" t="n">
+        <v>93</v>
+      </c>
+      <c r="E35" s="99" t="n">
+        <v>20</v>
       </c>
       <c r="F35" s="95" t="n">
-        <v>21</v>
+        <v>338</v>
       </c>
       <c r="G35" s="100" t="inlineStr">
         <is>
@@ -3780,42 +3717,42 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K35" s="102" t="inlineStr">
-        <is>
-          <t>45</t>
+      <c r="K35" s="106" t="inlineStr">
+        <is>
+          <t>11.8</t>
         </is>
       </c>
       <c r="L35" s="100" t="inlineStr">
         <is>
-          <t>1.7</t>
-        </is>
-      </c>
-      <c r="M35" s="95" t="inlineStr">
-        <is>
-          <t>0</t>
+          <t>0.8</t>
+        </is>
+      </c>
+      <c r="M35" s="100" t="inlineStr">
+        <is>
+          <t>1.6</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="95" t="inlineStr">
         <is>
-          <t>2021-12-18 21:00 sab</t>
-        </is>
-      </c>
-      <c r="B36" s="97" t="n">
-        <v>7</v>
-      </c>
-      <c r="C36" s="97" t="n">
-        <v>-3</v>
-      </c>
-      <c r="D36" s="98" t="n">
-        <v>45</v>
+          <t xml:space="preserve">2022-01-02 09:00 Sun Sun </t>
+        </is>
+      </c>
+      <c r="B36" s="98" t="n">
+        <v>14</v>
+      </c>
+      <c r="C36" s="107" t="n">
+        <v>11</v>
+      </c>
+      <c r="D36" s="104" t="n">
+        <v>81</v>
       </c>
       <c r="E36" s="98" t="n">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F36" s="95" t="n">
-        <v>30</v>
+        <v>346</v>
       </c>
       <c r="G36" s="100" t="inlineStr">
         <is>
@@ -3837,14 +3774,14 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K36" s="102" t="inlineStr">
-        <is>
-          <t>42.6</t>
-        </is>
-      </c>
-      <c r="L36" s="102" t="inlineStr">
-        <is>
-          <t>36</t>
+      <c r="K36" s="106" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="L36" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="M36" s="95" t="inlineStr">
@@ -3856,23 +3793,23 @@
     <row r="37">
       <c r="A37" s="95" t="inlineStr">
         <is>
-          <t>2021-12-19 00:00 dom</t>
-        </is>
-      </c>
-      <c r="B37" s="97" t="n">
-        <v>7</v>
-      </c>
-      <c r="C37" s="97" t="n">
-        <v>-3</v>
-      </c>
-      <c r="D37" s="98" t="n">
-        <v>47</v>
+          <t xml:space="preserve">2022-01-02 12:00 Sun Sun </t>
+        </is>
+      </c>
+      <c r="B37" s="98" t="n">
+        <v>15</v>
+      </c>
+      <c r="C37" s="98" t="n">
+        <v>10</v>
+      </c>
+      <c r="D37" s="104" t="n">
+        <v>72</v>
       </c>
       <c r="E37" s="98" t="n">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F37" s="95" t="n">
-        <v>25</v>
+        <v>344</v>
       </c>
       <c r="G37" s="100" t="inlineStr">
         <is>
@@ -3894,14 +3831,14 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K37" s="101" t="inlineStr">
-        <is>
-          <t>23.8</t>
-        </is>
-      </c>
-      <c r="L37" s="102" t="inlineStr">
-        <is>
-          <t>32.3</t>
+      <c r="K37" s="106" t="inlineStr">
+        <is>
+          <t>10.2</t>
+        </is>
+      </c>
+      <c r="L37" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="M37" s="95" t="inlineStr">
@@ -3913,23 +3850,23 @@
     <row r="38">
       <c r="A38" s="95" t="inlineStr">
         <is>
-          <t>2021-12-19 03:00 dom</t>
-        </is>
-      </c>
-      <c r="B38" s="97" t="n">
-        <v>6</v>
-      </c>
-      <c r="C38" s="97" t="n">
-        <v>-2</v>
-      </c>
-      <c r="D38" s="98" t="n">
-        <v>51</v>
-      </c>
-      <c r="E38" s="98" t="n">
-        <v>30</v>
+          <t xml:space="preserve">2022-01-02 15:00 Sun Sun </t>
+        </is>
+      </c>
+      <c r="B38" s="101" t="n">
+        <v>13</v>
+      </c>
+      <c r="C38" s="98" t="n">
+        <v>10</v>
+      </c>
+      <c r="D38" s="104" t="n">
+        <v>84</v>
+      </c>
+      <c r="E38" s="99" t="n">
+        <v>16</v>
       </c>
       <c r="F38" s="95" t="n">
-        <v>26</v>
+        <v>345</v>
       </c>
       <c r="G38" s="100" t="inlineStr">
         <is>
@@ -3951,42 +3888,42 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K38" s="100" t="inlineStr">
-        <is>
-          <t>3.8</t>
-        </is>
-      </c>
-      <c r="L38" s="102" t="inlineStr">
-        <is>
-          <t>45.3</t>
-        </is>
-      </c>
-      <c r="M38" s="95" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K38" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L38" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M38" s="100" t="inlineStr">
+        <is>
+          <t>3.3</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="95" t="inlineStr">
         <is>
-          <t>2021-12-19 06:00 dom</t>
-        </is>
-      </c>
-      <c r="B39" s="97" t="n">
-        <v>6</v>
-      </c>
-      <c r="C39" s="97" t="n">
-        <v>-3</v>
-      </c>
-      <c r="D39" s="98" t="n">
-        <v>50</v>
-      </c>
-      <c r="E39" s="98" t="n">
-        <v>28</v>
+          <t xml:space="preserve">2022-01-02 18:00 Sun Sun </t>
+        </is>
+      </c>
+      <c r="B39" s="101" t="n">
+        <v>11</v>
+      </c>
+      <c r="C39" s="98" t="n">
+        <v>10</v>
+      </c>
+      <c r="D39" s="104" t="n">
+        <v>94</v>
+      </c>
+      <c r="E39" s="100" t="n">
+        <v>9</v>
       </c>
       <c r="F39" s="95" t="n">
-        <v>19</v>
+        <v>332</v>
       </c>
       <c r="G39" s="100" t="inlineStr">
         <is>
@@ -4008,42 +3945,42 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K39" s="100" t="inlineStr">
-        <is>
-          <t>4.4</t>
-        </is>
-      </c>
-      <c r="L39" s="101" t="inlineStr">
-        <is>
-          <t>23.5</t>
-        </is>
-      </c>
-      <c r="M39" s="95" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K39" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L39" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M39" s="108" t="inlineStr">
+        <is>
+          <t>5.7</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="95" t="inlineStr">
         <is>
-          <t>2021-12-19 09:00 dom</t>
+          <t xml:space="preserve">2022-01-02 21:00 Sun Sun </t>
         </is>
       </c>
       <c r="B40" s="97" t="n">
-        <v>8</v>
-      </c>
-      <c r="C40" s="97" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D40" s="98" t="n">
-        <v>49</v>
-      </c>
-      <c r="E40" s="98" t="n">
-        <v>30</v>
+        <v>10</v>
+      </c>
+      <c r="C40" s="98" t="n">
+        <v>9</v>
+      </c>
+      <c r="D40" s="104" t="n">
+        <v>92</v>
+      </c>
+      <c r="E40" s="100" t="n">
+        <v>5</v>
       </c>
       <c r="F40" s="95" t="n">
-        <v>21</v>
+        <v>321</v>
       </c>
       <c r="G40" s="100" t="inlineStr">
         <is>
@@ -4065,42 +4002,42 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K40" s="100" t="inlineStr">
+      <c r="K40" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L40" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M40" s="108" t="inlineStr">
         <is>
           <t>5</t>
-        </is>
-      </c>
-      <c r="L40" s="95" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="M40" s="95" t="inlineStr">
-        <is>
-          <t>0</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="95" t="inlineStr">
         <is>
-          <t>2021-12-19 12:00 dom</t>
+          <t xml:space="preserve">2022-01-03 00:00 Mon Mon </t>
         </is>
       </c>
       <c r="B41" s="97" t="n">
-        <v>8</v>
-      </c>
-      <c r="C41" s="97" t="n">
-        <v>-1</v>
-      </c>
-      <c r="D41" s="98" t="n">
-        <v>49</v>
-      </c>
-      <c r="E41" s="98" t="n">
-        <v>37</v>
+        <v>9</v>
+      </c>
+      <c r="C41" s="98" t="n">
+        <v>7</v>
+      </c>
+      <c r="D41" s="104" t="n">
+        <v>89</v>
+      </c>
+      <c r="E41" s="100" t="n">
+        <v>1</v>
       </c>
       <c r="F41" s="95" t="n">
-        <v>7</v>
+        <v>338</v>
       </c>
       <c r="G41" s="100" t="inlineStr">
         <is>
@@ -4122,9 +4059,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K41" s="100" t="inlineStr">
-        <is>
-          <t>5</t>
+      <c r="K41" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L41" s="95" t="inlineStr">
@@ -4132,32 +4069,32 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M41" s="95" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M41" s="108" t="inlineStr">
+        <is>
+          <t>6.4</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="95" t="inlineStr">
         <is>
-          <t>2021-12-19 15:00 dom</t>
+          <t xml:space="preserve">2022-01-03 03:00 Mon Mon </t>
         </is>
       </c>
       <c r="B42" s="97" t="n">
+        <v>9</v>
+      </c>
+      <c r="C42" s="98" t="n">
         <v>7</v>
       </c>
-      <c r="C42" s="97" t="n">
-        <v>-2</v>
-      </c>
-      <c r="D42" s="98" t="n">
-        <v>50</v>
-      </c>
-      <c r="E42" s="98" t="n">
-        <v>34</v>
+      <c r="D42" s="104" t="n">
+        <v>86</v>
+      </c>
+      <c r="E42" s="100" t="n">
+        <v>3</v>
       </c>
       <c r="F42" s="95" t="n">
-        <v>15</v>
+        <v>130</v>
       </c>
       <c r="G42" s="100" t="inlineStr">
         <is>
@@ -4179,9 +4116,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K42" s="100" t="inlineStr">
-        <is>
-          <t>5</t>
+      <c r="K42" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L42" s="95" t="inlineStr">
@@ -4189,32 +4126,32 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M42" s="95" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M42" s="108" t="inlineStr">
+        <is>
+          <t>5.4</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="95" t="inlineStr">
         <is>
-          <t>2021-12-19 18:00 dom</t>
+          <t xml:space="preserve">2022-01-03 06:00 Mon Mon </t>
         </is>
       </c>
       <c r="B43" s="97" t="n">
+        <v>9</v>
+      </c>
+      <c r="C43" s="98" t="n">
         <v>6</v>
       </c>
-      <c r="C43" s="97" t="n">
-        <v>-2</v>
-      </c>
-      <c r="D43" s="98" t="n">
-        <v>49</v>
-      </c>
-      <c r="E43" s="98" t="n">
-        <v>24</v>
+      <c r="D43" s="104" t="n">
+        <v>85</v>
+      </c>
+      <c r="E43" s="100" t="n">
+        <v>5</v>
       </c>
       <c r="F43" s="95" t="n">
-        <v>0</v>
+        <v>159</v>
       </c>
       <c r="G43" s="100" t="inlineStr">
         <is>
@@ -4236,9 +4173,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K43" s="100" t="inlineStr">
-        <is>
-          <t>4.7</t>
+      <c r="K43" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L43" s="95" t="inlineStr">
@@ -4246,32 +4183,32 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M43" s="95" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M43" s="108" t="inlineStr">
+        <is>
+          <t>6.5</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="95" t="inlineStr">
         <is>
-          <t>2021-12-19 21:00 dom</t>
-        </is>
-      </c>
-      <c r="B44" s="97" t="n">
-        <v>6</v>
-      </c>
-      <c r="C44" s="97" t="n">
-        <v>-2</v>
-      </c>
-      <c r="D44" s="98" t="n">
-        <v>53</v>
-      </c>
-      <c r="E44" s="99" t="n">
-        <v>16</v>
+          <t xml:space="preserve">2022-01-03 09:00 Mon Mon </t>
+        </is>
+      </c>
+      <c r="B44" s="101" t="n">
+        <v>13</v>
+      </c>
+      <c r="C44" s="98" t="n">
+        <v>8</v>
+      </c>
+      <c r="D44" s="104" t="n">
+        <v>73</v>
+      </c>
+      <c r="E44" s="100" t="n">
+        <v>3</v>
       </c>
       <c r="F44" s="95" t="n">
-        <v>340</v>
+        <v>96</v>
       </c>
       <c r="G44" s="100" t="inlineStr">
         <is>
@@ -4293,9 +4230,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K44" s="100" t="inlineStr">
-        <is>
-          <t>3.9</t>
+      <c r="K44" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L44" s="95" t="inlineStr">
@@ -4303,32 +4240,32 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M44" s="95" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M44" s="103" t="inlineStr">
+        <is>
+          <t>73.7</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="95" t="inlineStr">
         <is>
-          <t>2021-12-20 00:00 lun</t>
-        </is>
-      </c>
-      <c r="B45" s="97" t="n">
-        <v>6</v>
-      </c>
-      <c r="C45" s="97" t="n">
-        <v>0</v>
+          <t xml:space="preserve">2022-01-03 12:00 Mon Mon </t>
+        </is>
+      </c>
+      <c r="B45" s="98" t="n">
+        <v>15</v>
+      </c>
+      <c r="C45" s="98" t="n">
+        <v>9</v>
       </c>
       <c r="D45" s="97" t="n">
-        <v>64</v>
-      </c>
-      <c r="E45" s="99" t="n">
-        <v>19</v>
+        <v>66</v>
+      </c>
+      <c r="E45" s="100" t="n">
+        <v>8</v>
       </c>
       <c r="F45" s="95" t="n">
-        <v>330</v>
+        <v>58</v>
       </c>
       <c r="G45" s="100" t="inlineStr">
         <is>
@@ -4350,9 +4287,9 @@
           <t>0</t>
         </is>
       </c>
-      <c r="K45" s="100" t="inlineStr">
-        <is>
-          <t>4.5</t>
+      <c r="K45" s="95" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
       <c r="L45" s="95" t="inlineStr">
@@ -4360,14 +4297,14 @@
           <t>0</t>
         </is>
       </c>
-      <c r="M45" s="95" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M45" s="102" t="inlineStr">
+        <is>
+          <t>54.6</t>
         </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>